<commit_message>
Another small update to WBS
</commit_message>
<xml_diff>
--- a/project/Work breakdown structure.xlsx
+++ b/project/Work breakdown structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\ES\Projects\SE2122-57672-58175-57957-58210-57911\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE024B57-903F-42DD-B63D-4F76D711B1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C2DB73-16E1-485E-9BD2-4DFDC88E9638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,21 +141,6 @@
     <t>W1</t>
   </si>
   <si>
-    <t>1.1 Create repository</t>
-  </si>
-  <si>
-    <t>1.4 Build Burnout Chart</t>
-  </si>
-  <si>
-    <t>1.3 Build WBS</t>
-  </si>
-  <si>
-    <t>1.2 Decide Scrum Masters</t>
-  </si>
-  <si>
-    <t>1.5 Divide tasks</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -235,6 +220,21 @@
   </si>
   <si>
     <t>During this time period we agreed not not work on the project as we had many other evalutations and projects.</t>
+  </si>
+  <si>
+    <t>Create repository</t>
+  </si>
+  <si>
+    <t>Decide Scrum Masters</t>
+  </si>
+  <si>
+    <t>Build WBS</t>
+  </si>
+  <si>
+    <t>Build Burnout Chart</t>
+  </si>
+  <si>
+    <t>Divide tasks</t>
   </si>
 </sst>
 </file>
@@ -1029,12 +1029,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1254,53 +1248,32 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1368,26 +1341,53 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1609,9 +1609,9 @@
   </sheetPr>
   <dimension ref="A1:AX1066"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T17" sqref="T17"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -1682,12 +1682,12 @@
     </row>
     <row r="2" spans="1:50" ht="14.25" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="107" t="s">
-        <v>41</v>
+      <c r="B2" s="98" t="s">
+        <v>36</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="109"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="6" spans="1:50" ht="14.25" customHeight="1" thickBot="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
@@ -2013,7 +2013,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2069,7 +2069,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2128,24 +2128,24 @@
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="91" t="s">
-        <v>66</v>
+      <c r="K10" s="129" t="s">
+        <v>61</v>
       </c>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="91"/>
-      <c r="S10" s="91"/>
-      <c r="T10" s="91"/>
-      <c r="U10" s="91"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="91"/>
-      <c r="X10" s="91"/>
-      <c r="Y10" s="91"/>
-      <c r="Z10" s="91"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="129"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="129"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="129"/>
+      <c r="S10" s="129"/>
+      <c r="T10" s="129"/>
+      <c r="U10" s="129"/>
+      <c r="V10" s="129"/>
+      <c r="W10" s="129"/>
+      <c r="X10" s="129"/>
+      <c r="Y10" s="129"/>
+      <c r="Z10" s="129"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -2173,1675 +2173,1685 @@
     </row>
     <row r="11" spans="1:50" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="129" t="s">
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="129" t="s">
+      <c r="G11" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="129" t="s">
+      <c r="H11" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="132" t="s">
+      <c r="I11" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="92" t="s">
+      <c r="J11" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="93"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="94"/>
-      <c r="Q11" s="92" t="s">
+      <c r="K11" s="131"/>
+      <c r="L11" s="131"/>
+      <c r="M11" s="131"/>
+      <c r="N11" s="131"/>
+      <c r="O11" s="131"/>
+      <c r="P11" s="132"/>
+      <c r="Q11" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="93"/>
-      <c r="S11" s="93"/>
-      <c r="T11" s="93"/>
-      <c r="U11" s="93"/>
-      <c r="V11" s="93"/>
-      <c r="W11" s="94"/>
-      <c r="X11" s="92" t="s">
+      <c r="R11" s="131"/>
+      <c r="S11" s="131"/>
+      <c r="T11" s="131"/>
+      <c r="U11" s="131"/>
+      <c r="V11" s="131"/>
+      <c r="W11" s="132"/>
+      <c r="X11" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="Y11" s="93"/>
-      <c r="Z11" s="93"/>
-      <c r="AA11" s="93"/>
-      <c r="AB11" s="93"/>
-      <c r="AC11" s="93"/>
-      <c r="AD11" s="94"/>
-      <c r="AE11" s="92" t="s">
+      <c r="Y11" s="131"/>
+      <c r="Z11" s="131"/>
+      <c r="AA11" s="131"/>
+      <c r="AB11" s="131"/>
+      <c r="AC11" s="131"/>
+      <c r="AD11" s="132"/>
+      <c r="AE11" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="AF11" s="93"/>
-      <c r="AG11" s="93"/>
-      <c r="AH11" s="93"/>
-      <c r="AI11" s="93"/>
-      <c r="AJ11" s="93"/>
-      <c r="AK11" s="94"/>
-      <c r="AL11" s="135"/>
-      <c r="AM11" s="135"/>
-      <c r="AN11" s="135"/>
-      <c r="AO11" s="135"/>
-      <c r="AP11" s="135"/>
-      <c r="AQ11" s="135"/>
-      <c r="AR11" s="95"/>
-      <c r="AS11" s="95"/>
-      <c r="AT11" s="95"/>
-      <c r="AU11" s="95"/>
-      <c r="AV11" s="95"/>
-      <c r="AW11" s="95"/>
-      <c r="AX11" s="95"/>
+      <c r="AF11" s="131"/>
+      <c r="AG11" s="131"/>
+      <c r="AH11" s="131"/>
+      <c r="AI11" s="131"/>
+      <c r="AJ11" s="131"/>
+      <c r="AK11" s="132"/>
+      <c r="AL11" s="97"/>
+      <c r="AM11" s="97"/>
+      <c r="AN11" s="97"/>
+      <c r="AO11" s="97"/>
+      <c r="AP11" s="97"/>
+      <c r="AQ11" s="97"/>
+      <c r="AR11" s="133"/>
+      <c r="AS11" s="133"/>
+      <c r="AT11" s="133"/>
+      <c r="AU11" s="133"/>
+      <c r="AV11" s="133"/>
+      <c r="AW11" s="133"/>
+      <c r="AX11" s="133"/>
     </row>
     <row r="12" spans="1:50" ht="14.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="26" t="s">
+      <c r="B12" s="115"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="26" t="s">
+      <c r="Q12" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="24" t="s">
+      <c r="R12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="24" t="s">
+      <c r="S12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="24" t="s">
+      <c r="T12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="24" t="s">
+      <c r="U12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="V12" s="24" t="s">
+      <c r="V12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="W12" s="27" t="s">
+      <c r="W12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="X12" s="26" t="s">
+      <c r="X12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Y12" s="24" t="s">
+      <c r="Y12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Z12" s="24" t="s">
+      <c r="Z12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AA12" s="24" t="s">
+      <c r="AA12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AB12" s="24" t="s">
+      <c r="AB12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC12" s="24" t="s">
+      <c r="AC12" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD12" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE12" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG12" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH12" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AD12" s="27" t="s">
+      <c r="AI12" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AE12" s="26" t="s">
+      <c r="AJ12" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="AF12" s="24" t="s">
+      <c r="AK12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AG12" s="24" t="s">
-        <v>61</v>
+      <c r="AL12" s="97"/>
+      <c r="AM12" s="97"/>
+      <c r="AN12" s="97"/>
+      <c r="AO12" s="97"/>
+      <c r="AP12" s="97"/>
+      <c r="AQ12" s="97"/>
+      <c r="AR12" s="133"/>
+      <c r="AS12" s="133"/>
+      <c r="AT12" s="133"/>
+      <c r="AU12" s="133"/>
+      <c r="AV12" s="133"/>
+      <c r="AW12" s="133"/>
+      <c r="AX12" s="133"/>
+    </row>
+    <row r="13" spans="1:50" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="26">
+        <v>44510</v>
       </c>
-      <c r="AH12" s="24" t="s">
+      <c r="K13" s="17">
+        <v>44511</v>
+      </c>
+      <c r="L13" s="17">
+        <v>44512</v>
+      </c>
+      <c r="M13" s="17">
+        <v>44513</v>
+      </c>
+      <c r="N13" s="17">
+        <v>44514</v>
+      </c>
+      <c r="O13" s="17">
+        <v>44515</v>
+      </c>
+      <c r="P13" s="27">
+        <v>44516</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>44517</v>
+      </c>
+      <c r="R13" s="17">
+        <v>44518</v>
+      </c>
+      <c r="S13" s="17">
+        <v>44519</v>
+      </c>
+      <c r="T13" s="17">
+        <v>44520</v>
+      </c>
+      <c r="U13" s="17">
+        <v>44521</v>
+      </c>
+      <c r="V13" s="17">
+        <v>44522</v>
+      </c>
+      <c r="W13" s="27">
+        <v>44523</v>
+      </c>
+      <c r="X13" s="26">
+        <v>44524</v>
+      </c>
+      <c r="Y13" s="17">
+        <v>44525</v>
+      </c>
+      <c r="Z13" s="17">
+        <v>44526</v>
+      </c>
+      <c r="AA13" s="17">
+        <v>44527</v>
+      </c>
+      <c r="AB13" s="17">
+        <v>44528</v>
+      </c>
+      <c r="AC13" s="17">
+        <v>44529</v>
+      </c>
+      <c r="AD13" s="27">
+        <v>44530</v>
+      </c>
+      <c r="AE13" s="26">
+        <v>44531</v>
+      </c>
+      <c r="AF13" s="17">
+        <v>44532</v>
+      </c>
+      <c r="AG13" s="17">
+        <v>44533</v>
+      </c>
+      <c r="AH13" s="17">
+        <v>44534</v>
+      </c>
+      <c r="AI13" s="17">
+        <v>44535</v>
+      </c>
+      <c r="AJ13" s="17">
+        <v>44536</v>
+      </c>
+      <c r="AK13" s="27">
+        <v>44537</v>
+      </c>
+      <c r="AL13" s="97"/>
+      <c r="AM13" s="97"/>
+      <c r="AN13" s="97"/>
+      <c r="AO13" s="97"/>
+      <c r="AP13" s="97"/>
+      <c r="AQ13" s="97"/>
+      <c r="AR13" s="133"/>
+      <c r="AS13" s="133"/>
+      <c r="AT13" s="133"/>
+      <c r="AU13" s="133"/>
+      <c r="AV13" s="133"/>
+      <c r="AW13" s="133"/>
+      <c r="AX13" s="133"/>
+    </row>
+    <row r="14" spans="1:50" ht="16.5" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="39"/>
+      <c r="AD14" s="40"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AI14" s="38"/>
+      <c r="AJ14" s="39"/>
+      <c r="AK14" s="40"/>
+      <c r="AL14" s="97"/>
+      <c r="AM14" s="97"/>
+      <c r="AN14" s="97"/>
+      <c r="AO14" s="97"/>
+      <c r="AP14" s="97"/>
+      <c r="AQ14" s="97"/>
+      <c r="AR14" s="133"/>
+      <c r="AS14" s="133"/>
+      <c r="AT14" s="133"/>
+      <c r="AU14" s="133"/>
+      <c r="AV14" s="133"/>
+      <c r="AW14" s="133"/>
+      <c r="AX14" s="133"/>
+    </row>
+    <row r="15" spans="1:50" s="11" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="134">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C15" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="AI12" s="24" t="s">
+      <c r="D15" s="108"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="20">
+        <v>44510</v>
+      </c>
+      <c r="G15" s="20">
+        <v>44510</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="86"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="52"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="52"/>
+      <c r="AA15" s="52"/>
+      <c r="AB15" s="52"/>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="45"/>
+      <c r="AF15" s="44"/>
+      <c r="AG15" s="52"/>
+      <c r="AH15" s="52"/>
+      <c r="AI15" s="52"/>
+      <c r="AJ15" s="46"/>
+      <c r="AK15" s="47"/>
+      <c r="AL15" s="97"/>
+      <c r="AM15" s="97"/>
+      <c r="AN15" s="97"/>
+      <c r="AO15" s="97"/>
+      <c r="AP15" s="97"/>
+      <c r="AQ15" s="97"/>
+      <c r="AR15" s="133"/>
+      <c r="AS15" s="133"/>
+      <c r="AT15" s="133"/>
+      <c r="AU15" s="133"/>
+      <c r="AV15" s="133"/>
+      <c r="AW15" s="133"/>
+      <c r="AX15" s="133"/>
+    </row>
+    <row r="16" spans="1:50" s="11" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A16" s="10"/>
+      <c r="B16" s="134">
+        <v>1.2</v>
+      </c>
+      <c r="C16" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="AJ12" s="24" t="s">
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="20">
+        <v>44510</v>
+      </c>
+      <c r="G16" s="20">
+        <v>44510</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="86"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="52"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="52"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="52"/>
+      <c r="AA16" s="52"/>
+      <c r="AB16" s="52"/>
+      <c r="AC16" s="46"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="45"/>
+      <c r="AF16" s="44"/>
+      <c r="AG16" s="52"/>
+      <c r="AH16" s="52"/>
+      <c r="AI16" s="52"/>
+      <c r="AJ16" s="46"/>
+      <c r="AK16" s="47"/>
+      <c r="AL16" s="97"/>
+      <c r="AM16" s="97"/>
+      <c r="AN16" s="97"/>
+      <c r="AO16" s="97"/>
+      <c r="AP16" s="97"/>
+      <c r="AQ16" s="97"/>
+      <c r="AR16" s="133"/>
+      <c r="AS16" s="133"/>
+      <c r="AT16" s="133"/>
+      <c r="AU16" s="133"/>
+      <c r="AV16" s="133"/>
+      <c r="AW16" s="133"/>
+      <c r="AX16" s="133"/>
+    </row>
+    <row r="17" spans="1:50" ht="14.25" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="134">
+        <v>1.3</v>
+      </c>
+      <c r="C17" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="AK12" s="27" t="s">
+      <c r="D17" s="108"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="21">
+        <v>44535</v>
+      </c>
+      <c r="G17" s="21">
+        <v>44535</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="44"/>
+      <c r="AA17" s="44"/>
+      <c r="AB17" s="44"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="45"/>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="44"/>
+      <c r="AH17" s="44"/>
+      <c r="AI17" s="88"/>
+      <c r="AJ17" s="23"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="97"/>
+      <c r="AM17" s="97"/>
+      <c r="AN17" s="97"/>
+      <c r="AO17" s="97"/>
+      <c r="AP17" s="97"/>
+      <c r="AQ17" s="97"/>
+      <c r="AR17" s="133"/>
+      <c r="AS17" s="133"/>
+      <c r="AT17" s="133"/>
+      <c r="AU17" s="133"/>
+      <c r="AV17" s="133"/>
+      <c r="AW17" s="133"/>
+      <c r="AX17" s="133"/>
+    </row>
+    <row r="18" spans="1:50" ht="14.25" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="134">
+        <v>1.4</v>
+      </c>
+      <c r="C18" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="AL12" s="135"/>
-      <c r="AM12" s="135"/>
-      <c r="AN12" s="135"/>
-      <c r="AO12" s="135"/>
-      <c r="AP12" s="135"/>
-      <c r="AQ12" s="135"/>
-      <c r="AR12" s="95"/>
-      <c r="AS12" s="95"/>
-      <c r="AT12" s="95"/>
-      <c r="AU12" s="95"/>
-      <c r="AV12" s="95"/>
-      <c r="AW12" s="95"/>
-      <c r="AX12" s="95"/>
-    </row>
-    <row r="13" spans="1:50" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="127"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="131"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="28">
-        <v>44510</v>
-      </c>
-      <c r="K13" s="19">
-        <v>44511</v>
-      </c>
-      <c r="L13" s="19">
-        <v>44512</v>
-      </c>
-      <c r="M13" s="19">
-        <v>44513</v>
-      </c>
-      <c r="N13" s="19">
-        <v>44514</v>
-      </c>
-      <c r="O13" s="19">
-        <v>44515</v>
-      </c>
-      <c r="P13" s="29">
-        <v>44516</v>
-      </c>
-      <c r="Q13" s="28">
-        <v>44517</v>
-      </c>
-      <c r="R13" s="19">
-        <v>44518</v>
-      </c>
-      <c r="S13" s="19">
-        <v>44519</v>
-      </c>
-      <c r="T13" s="19">
-        <v>44520</v>
-      </c>
-      <c r="U13" s="19">
-        <v>44521</v>
-      </c>
-      <c r="V13" s="19">
-        <v>44522</v>
-      </c>
-      <c r="W13" s="29">
-        <v>44523</v>
-      </c>
-      <c r="X13" s="28">
-        <v>44524</v>
-      </c>
-      <c r="Y13" s="19">
-        <v>44525</v>
-      </c>
-      <c r="Z13" s="19">
-        <v>44526</v>
-      </c>
-      <c r="AA13" s="19">
-        <v>44527</v>
-      </c>
-      <c r="AB13" s="19">
-        <v>44528</v>
-      </c>
-      <c r="AC13" s="19">
-        <v>44529</v>
-      </c>
-      <c r="AD13" s="29">
-        <v>44530</v>
-      </c>
-      <c r="AE13" s="28">
-        <v>44531</v>
-      </c>
-      <c r="AF13" s="19">
-        <v>44532</v>
-      </c>
-      <c r="AG13" s="19">
-        <v>44533</v>
-      </c>
-      <c r="AH13" s="19">
-        <v>44534</v>
-      </c>
-      <c r="AI13" s="19">
+      <c r="D18" s="108"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="21">
         <v>44535</v>
       </c>
-      <c r="AJ13" s="19">
-        <v>44536</v>
+      <c r="G18" s="21">
+        <v>44535</v>
       </c>
-      <c r="AK13" s="29">
-        <v>44537</v>
+      <c r="H18" s="16" t="s">
+        <v>35</v>
       </c>
-      <c r="AL13" s="135"/>
-      <c r="AM13" s="135"/>
-      <c r="AN13" s="135"/>
-      <c r="AO13" s="135"/>
-      <c r="AP13" s="135"/>
-      <c r="AQ13" s="135"/>
-      <c r="AR13" s="95"/>
-      <c r="AS13" s="95"/>
-      <c r="AT13" s="95"/>
-      <c r="AU13" s="95"/>
-      <c r="AV13" s="95"/>
-      <c r="AW13" s="95"/>
-      <c r="AX13" s="95"/>
-    </row>
-    <row r="14" spans="1:50" ht="16.5" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="51" t="s">
+      <c r="I18" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="39"/>
-      <c r="Y14" s="40"/>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="40"/>
-      <c r="AB14" s="40"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="42"/>
-      <c r="AE14" s="39"/>
-      <c r="AF14" s="40"/>
-      <c r="AG14" s="40"/>
-      <c r="AH14" s="40"/>
-      <c r="AI14" s="40"/>
-      <c r="AJ14" s="41"/>
-      <c r="AK14" s="42"/>
-      <c r="AL14" s="135"/>
-      <c r="AM14" s="135"/>
-      <c r="AN14" s="135"/>
-      <c r="AO14" s="135"/>
-      <c r="AP14" s="135"/>
-      <c r="AQ14" s="135"/>
-      <c r="AR14" s="95"/>
-      <c r="AS14" s="95"/>
-      <c r="AT14" s="95"/>
-      <c r="AU14" s="95"/>
-      <c r="AV14" s="95"/>
-      <c r="AW14" s="95"/>
-      <c r="AX14" s="95"/>
-    </row>
-    <row r="15" spans="1:50" s="11" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="101" t="s">
+      <c r="J18" s="45"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="44"/>
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="45"/>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="23"/>
+      <c r="AH18" s="23"/>
+      <c r="AI18" s="84"/>
+      <c r="AJ18" s="44"/>
+      <c r="AK18" s="48"/>
+      <c r="AL18" s="97"/>
+      <c r="AM18" s="97"/>
+      <c r="AN18" s="97"/>
+      <c r="AO18" s="97"/>
+      <c r="AP18" s="97"/>
+      <c r="AQ18" s="97"/>
+      <c r="AR18" s="133"/>
+      <c r="AS18" s="133"/>
+      <c r="AT18" s="133"/>
+      <c r="AU18" s="133"/>
+      <c r="AV18" s="133"/>
+      <c r="AW18" s="133"/>
+      <c r="AX18" s="133"/>
+    </row>
+    <row r="19" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="135">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="111"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="21">
+        <v>44535</v>
+      </c>
+      <c r="G19" s="21">
+        <v>44535</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="117"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="22">
-        <v>44510</v>
-      </c>
-      <c r="G15" s="22">
-        <v>44510</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="52" t="s">
+      <c r="I19" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="88"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="49"/>
-      <c r="X15" s="47"/>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
-      <c r="AB15" s="54"/>
-      <c r="AC15" s="48"/>
-      <c r="AD15" s="49"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="46"/>
-      <c r="AG15" s="54"/>
-      <c r="AH15" s="54"/>
-      <c r="AI15" s="54"/>
-      <c r="AJ15" s="48"/>
-      <c r="AK15" s="49"/>
-      <c r="AL15" s="135"/>
-      <c r="AM15" s="135"/>
-      <c r="AN15" s="135"/>
-      <c r="AO15" s="135"/>
-      <c r="AP15" s="135"/>
-      <c r="AQ15" s="135"/>
-      <c r="AR15" s="95"/>
-      <c r="AS15" s="95"/>
-      <c r="AT15" s="95"/>
-      <c r="AU15" s="95"/>
-      <c r="AV15" s="95"/>
-      <c r="AW15" s="95"/>
-      <c r="AX15" s="95"/>
-    </row>
-    <row r="16" spans="1:50" s="11" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="101" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="22">
-        <v>44510</v>
-      </c>
-      <c r="G16" s="22">
-        <v>44510</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="88"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="54"/>
-      <c r="T16" s="54"/>
-      <c r="U16" s="54"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="49"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="46"/>
-      <c r="Z16" s="54"/>
-      <c r="AA16" s="54"/>
-      <c r="AB16" s="54"/>
-      <c r="AC16" s="48"/>
-      <c r="AD16" s="49"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="46"/>
-      <c r="AG16" s="54"/>
-      <c r="AH16" s="54"/>
-      <c r="AI16" s="54"/>
-      <c r="AJ16" s="48"/>
-      <c r="AK16" s="49"/>
-      <c r="AL16" s="135"/>
-      <c r="AM16" s="135"/>
-      <c r="AN16" s="135"/>
-      <c r="AO16" s="135"/>
-      <c r="AP16" s="135"/>
-      <c r="AQ16" s="135"/>
-      <c r="AR16" s="95"/>
-      <c r="AS16" s="95"/>
-      <c r="AT16" s="95"/>
-      <c r="AU16" s="95"/>
-      <c r="AV16" s="95"/>
-      <c r="AW16" s="95"/>
-      <c r="AX16" s="95"/>
-    </row>
-    <row r="17" spans="1:50" ht="14.25" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="117"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="23">
-        <v>44535</v>
-      </c>
-      <c r="G17" s="23">
-        <v>44535</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="47"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="46"/>
-      <c r="AB17" s="46"/>
-      <c r="AC17" s="25"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="46"/>
-      <c r="AH17" s="46"/>
-      <c r="AI17" s="90"/>
-      <c r="AJ17" s="25"/>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="135"/>
-      <c r="AM17" s="135"/>
-      <c r="AN17" s="135"/>
-      <c r="AO17" s="135"/>
-      <c r="AP17" s="135"/>
-      <c r="AQ17" s="135"/>
-      <c r="AR17" s="95"/>
-      <c r="AS17" s="95"/>
-      <c r="AT17" s="95"/>
-      <c r="AU17" s="95"/>
-      <c r="AV17" s="95"/>
-      <c r="AW17" s="95"/>
-      <c r="AX17" s="95"/>
-    </row>
-    <row r="18" spans="1:50" ht="14.25" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="117"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="23">
-        <v>44535</v>
-      </c>
-      <c r="G18" s="23">
-        <v>44535</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="47"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="46"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="47"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="46"/>
-      <c r="AD18" s="50"/>
-      <c r="AE18" s="47"/>
-      <c r="AF18" s="25"/>
-      <c r="AG18" s="25"/>
-      <c r="AH18" s="25"/>
-      <c r="AI18" s="86"/>
-      <c r="AJ18" s="46"/>
-      <c r="AK18" s="50"/>
-      <c r="AL18" s="135"/>
-      <c r="AM18" s="135"/>
-      <c r="AN18" s="135"/>
-      <c r="AO18" s="135"/>
-      <c r="AP18" s="135"/>
-      <c r="AQ18" s="135"/>
-      <c r="AR18" s="95"/>
-      <c r="AS18" s="95"/>
-      <c r="AT18" s="95"/>
-      <c r="AU18" s="95"/>
-      <c r="AV18" s="95"/>
-      <c r="AW18" s="95"/>
-      <c r="AX18" s="95"/>
-    </row>
-    <row r="19" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="119" t="s">
+      <c r="J19" s="45"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="45"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="23"/>
+      <c r="AI19" s="84"/>
+      <c r="AJ19" s="23"/>
+      <c r="AK19" s="29"/>
+      <c r="AL19" s="97"/>
+      <c r="AM19" s="97"/>
+      <c r="AN19" s="97"/>
+      <c r="AO19" s="97"/>
+      <c r="AP19" s="97"/>
+      <c r="AQ19" s="97"/>
+      <c r="AR19" s="133"/>
+      <c r="AS19" s="133"/>
+      <c r="AT19" s="133"/>
+      <c r="AU19" s="133"/>
+      <c r="AV19" s="133"/>
+      <c r="AW19" s="133"/>
+      <c r="AX19" s="133"/>
+    </row>
+    <row r="20" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="120"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="23">
-        <v>44535</v>
-      </c>
-      <c r="G19" s="23">
-        <v>44535</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="25"/>
-      <c r="Z19" s="25"/>
-      <c r="AA19" s="25"/>
-      <c r="AB19" s="25"/>
-      <c r="AC19" s="25"/>
-      <c r="AD19" s="31"/>
-      <c r="AE19" s="47"/>
-      <c r="AF19" s="25"/>
-      <c r="AG19" s="25"/>
-      <c r="AH19" s="25"/>
-      <c r="AI19" s="86"/>
-      <c r="AJ19" s="25"/>
-      <c r="AK19" s="31"/>
-      <c r="AL19" s="135"/>
-      <c r="AM19" s="135"/>
-      <c r="AN19" s="135"/>
-      <c r="AO19" s="135"/>
-      <c r="AP19" s="135"/>
-      <c r="AQ19" s="135"/>
-      <c r="AR19" s="95"/>
-      <c r="AS19" s="95"/>
-      <c r="AT19" s="95"/>
-      <c r="AU19" s="95"/>
-      <c r="AV19" s="95"/>
-      <c r="AW19" s="95"/>
-      <c r="AX19" s="95"/>
-    </row>
-    <row r="20" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="113" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="44"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="39"/>
-      <c r="Y20" s="44"/>
-      <c r="Z20" s="44"/>
-      <c r="AA20" s="44"/>
-      <c r="AB20" s="44"/>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="45"/>
-      <c r="AE20" s="39"/>
-      <c r="AF20" s="44"/>
-      <c r="AG20" s="44"/>
-      <c r="AH20" s="44"/>
-      <c r="AI20" s="44"/>
-      <c r="AJ20" s="44"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="135"/>
-      <c r="AM20" s="135"/>
-      <c r="AN20" s="135"/>
-      <c r="AO20" s="135"/>
-      <c r="AP20" s="135"/>
-      <c r="AQ20" s="135"/>
-      <c r="AR20" s="95"/>
-      <c r="AS20" s="95"/>
-      <c r="AT20" s="95"/>
-      <c r="AU20" s="95"/>
-      <c r="AV20" s="95"/>
-      <c r="AW20" s="95"/>
-      <c r="AX20" s="95"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="43"/>
+      <c r="AE20" s="37"/>
+      <c r="AF20" s="42"/>
+      <c r="AG20" s="42"/>
+      <c r="AH20" s="42"/>
+      <c r="AI20" s="42"/>
+      <c r="AJ20" s="42"/>
+      <c r="AK20" s="43"/>
+      <c r="AL20" s="97"/>
+      <c r="AM20" s="97"/>
+      <c r="AN20" s="97"/>
+      <c r="AO20" s="97"/>
+      <c r="AP20" s="97"/>
+      <c r="AQ20" s="97"/>
+      <c r="AR20" s="133"/>
+      <c r="AS20" s="133"/>
+      <c r="AT20" s="133"/>
+      <c r="AU20" s="133"/>
+      <c r="AV20" s="133"/>
+      <c r="AW20" s="133"/>
+      <c r="AX20" s="133"/>
     </row>
     <row r="21" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="15">
         <v>2.0099999999999998</v>
       </c>
-      <c r="C21" s="100" t="s">
-        <v>46</v>
+      <c r="C21" s="89" t="s">
+        <v>41</v>
       </c>
-      <c r="D21" s="100"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="38">
+      <c r="D21" s="89"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="36">
         <v>44527</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="18">
         <v>44534</v>
       </c>
-      <c r="H21" s="21" t="s">
-        <v>40</v>
+      <c r="H21" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="86"/>
-      <c r="AB21" s="86"/>
-      <c r="AC21" s="86"/>
-      <c r="AD21" s="87"/>
-      <c r="AE21" s="88"/>
-      <c r="AF21" s="86"/>
-      <c r="AG21" s="86"/>
-      <c r="AH21" s="86"/>
-      <c r="AI21" s="25"/>
-      <c r="AJ21" s="25"/>
-      <c r="AK21" s="31"/>
-      <c r="AL21" s="135"/>
-      <c r="AM21" s="135"/>
-      <c r="AN21" s="135"/>
-      <c r="AO21" s="135"/>
-      <c r="AP21" s="135"/>
-      <c r="AQ21" s="135"/>
-      <c r="AR21" s="95"/>
-      <c r="AS21" s="95"/>
-      <c r="AT21" s="95"/>
-      <c r="AU21" s="95"/>
-      <c r="AV21" s="95"/>
-      <c r="AW21" s="95"/>
-      <c r="AX21" s="95"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="84"/>
+      <c r="AB21" s="84"/>
+      <c r="AC21" s="84"/>
+      <c r="AD21" s="85"/>
+      <c r="AE21" s="86"/>
+      <c r="AF21" s="84"/>
+      <c r="AG21" s="84"/>
+      <c r="AH21" s="84"/>
+      <c r="AI21" s="23"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="29"/>
+      <c r="AL21" s="97"/>
+      <c r="AM21" s="97"/>
+      <c r="AN21" s="97"/>
+      <c r="AO21" s="97"/>
+      <c r="AP21" s="97"/>
+      <c r="AQ21" s="97"/>
+      <c r="AR21" s="133"/>
+      <c r="AS21" s="133"/>
+      <c r="AT21" s="133"/>
+      <c r="AU21" s="133"/>
+      <c r="AV21" s="133"/>
+      <c r="AW21" s="133"/>
+      <c r="AX21" s="133"/>
     </row>
     <row r="22" spans="1:50" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="15">
         <v>2.02</v>
       </c>
-      <c r="C22" s="100" t="s">
-        <v>47</v>
+      <c r="C22" s="89" t="s">
+        <v>42</v>
       </c>
-      <c r="D22" s="100"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="38">
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="36">
         <v>44527</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="18">
         <v>44534</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>40</v>
+      <c r="H22" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="25"/>
-      <c r="V22" s="25"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="25"/>
-      <c r="AA22" s="86"/>
-      <c r="AB22" s="86"/>
-      <c r="AC22" s="86"/>
-      <c r="AD22" s="87"/>
-      <c r="AE22" s="88"/>
-      <c r="AF22" s="86"/>
-      <c r="AG22" s="86"/>
-      <c r="AH22" s="86"/>
-      <c r="AI22" s="25"/>
-      <c r="AJ22" s="25"/>
-      <c r="AK22" s="31"/>
-      <c r="AL22" s="135"/>
-      <c r="AM22" s="135"/>
-      <c r="AN22" s="135"/>
-      <c r="AO22" s="135"/>
-      <c r="AP22" s="135"/>
-      <c r="AQ22" s="135"/>
-      <c r="AR22" s="95"/>
-      <c r="AS22" s="95"/>
-      <c r="AT22" s="95"/>
-      <c r="AU22" s="95"/>
-      <c r="AV22" s="95"/>
-      <c r="AW22" s="95"/>
-      <c r="AX22" s="95"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="84"/>
+      <c r="AB22" s="84"/>
+      <c r="AC22" s="84"/>
+      <c r="AD22" s="85"/>
+      <c r="AE22" s="86"/>
+      <c r="AF22" s="84"/>
+      <c r="AG22" s="84"/>
+      <c r="AH22" s="84"/>
+      <c r="AI22" s="23"/>
+      <c r="AJ22" s="23"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="97"/>
+      <c r="AM22" s="97"/>
+      <c r="AN22" s="97"/>
+      <c r="AO22" s="97"/>
+      <c r="AP22" s="97"/>
+      <c r="AQ22" s="97"/>
+      <c r="AR22" s="133"/>
+      <c r="AS22" s="133"/>
+      <c r="AT22" s="133"/>
+      <c r="AU22" s="133"/>
+      <c r="AV22" s="133"/>
+      <c r="AW22" s="133"/>
+      <c r="AX22" s="133"/>
     </row>
     <row r="23" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="15">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C23" s="100" t="s">
-        <v>48</v>
+      <c r="C23" s="89" t="s">
+        <v>43</v>
       </c>
-      <c r="D23" s="100"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="38">
+      <c r="D23" s="89"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="36">
         <v>44533</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="18">
         <v>44534</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>40</v>
+      <c r="H23" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I23" s="52" t="s">
+      <c r="I23" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J23" s="30"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
-      <c r="AA23" s="25"/>
-      <c r="AB23" s="25"/>
-      <c r="AC23" s="25"/>
-      <c r="AD23" s="31"/>
-      <c r="AE23" s="30"/>
-      <c r="AF23" s="25"/>
-      <c r="AG23" s="86"/>
-      <c r="AH23" s="86"/>
-      <c r="AI23" s="25"/>
-      <c r="AJ23" s="25"/>
-      <c r="AK23" s="31"/>
-      <c r="AL23" s="135"/>
-      <c r="AM23" s="135"/>
-      <c r="AN23" s="135"/>
-      <c r="AO23" s="135"/>
-      <c r="AP23" s="135"/>
-      <c r="AQ23" s="135"/>
-      <c r="AR23" s="95"/>
-      <c r="AS23" s="95"/>
-      <c r="AT23" s="95"/>
-      <c r="AU23" s="95"/>
-      <c r="AV23" s="95"/>
-      <c r="AW23" s="95"/>
-      <c r="AX23" s="95"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="84"/>
+      <c r="AH23" s="84"/>
+      <c r="AI23" s="23"/>
+      <c r="AJ23" s="23"/>
+      <c r="AK23" s="29"/>
+      <c r="AL23" s="97"/>
+      <c r="AM23" s="97"/>
+      <c r="AN23" s="97"/>
+      <c r="AO23" s="97"/>
+      <c r="AP23" s="97"/>
+      <c r="AQ23" s="97"/>
+      <c r="AR23" s="133"/>
+      <c r="AS23" s="133"/>
+      <c r="AT23" s="133"/>
+      <c r="AU23" s="133"/>
+      <c r="AV23" s="133"/>
+      <c r="AW23" s="133"/>
+      <c r="AX23" s="133"/>
     </row>
     <row r="24" spans="1:50" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="15">
         <v>2.04</v>
       </c>
-      <c r="C24" s="100" t="s">
-        <v>49</v>
+      <c r="C24" s="89" t="s">
+        <v>44</v>
       </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="38">
+      <c r="D24" s="89"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="36">
         <v>44533</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="18">
         <v>44534</v>
       </c>
-      <c r="H24" s="21" t="s">
-        <v>40</v>
+      <c r="H24" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I24" s="52" t="s">
+      <c r="I24" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="30"/>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="86"/>
-      <c r="AH24" s="86"/>
-      <c r="AI24" s="25"/>
-      <c r="AJ24" s="25"/>
-      <c r="AK24" s="31"/>
-      <c r="AL24" s="135"/>
-      <c r="AM24" s="135"/>
-      <c r="AN24" s="135"/>
-      <c r="AO24" s="135"/>
-      <c r="AP24" s="135"/>
-      <c r="AQ24" s="135"/>
-      <c r="AR24" s="95"/>
-      <c r="AS24" s="95"/>
-      <c r="AT24" s="95"/>
-      <c r="AU24" s="95"/>
-      <c r="AV24" s="95"/>
-      <c r="AW24" s="95"/>
-      <c r="AX24" s="95"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="84"/>
+      <c r="AH24" s="84"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="23"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="97"/>
+      <c r="AM24" s="97"/>
+      <c r="AN24" s="97"/>
+      <c r="AO24" s="97"/>
+      <c r="AP24" s="97"/>
+      <c r="AQ24" s="97"/>
+      <c r="AR24" s="133"/>
+      <c r="AS24" s="133"/>
+      <c r="AT24" s="133"/>
+      <c r="AU24" s="133"/>
+      <c r="AV24" s="133"/>
+      <c r="AW24" s="133"/>
+      <c r="AX24" s="133"/>
     </row>
     <row r="25" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="15">
         <v>2.0499999999999998</v>
       </c>
-      <c r="C25" s="100" t="s">
-        <v>50</v>
+      <c r="C25" s="89" t="s">
+        <v>45</v>
       </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="38">
+      <c r="D25" s="89"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="36">
         <v>44533</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="18">
         <v>44534</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>40</v>
+      <c r="H25" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I25" s="53" t="s">
+      <c r="I25" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="25"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="25"/>
-      <c r="AC25" s="25"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="25"/>
-      <c r="AI25" s="86"/>
-      <c r="AJ25" s="25"/>
-      <c r="AK25" s="31"/>
-      <c r="AL25" s="135"/>
-      <c r="AM25" s="135"/>
-      <c r="AN25" s="135"/>
-      <c r="AO25" s="135"/>
-      <c r="AP25" s="135"/>
-      <c r="AQ25" s="135"/>
-      <c r="AR25" s="95"/>
-      <c r="AS25" s="95"/>
-      <c r="AT25" s="95"/>
-      <c r="AU25" s="95"/>
-      <c r="AV25" s="95"/>
-      <c r="AW25" s="95"/>
-      <c r="AX25" s="95"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
+      <c r="AC25" s="23"/>
+      <c r="AD25" s="29"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="84"/>
+      <c r="AJ25" s="23"/>
+      <c r="AK25" s="29"/>
+      <c r="AL25" s="97"/>
+      <c r="AM25" s="97"/>
+      <c r="AN25" s="97"/>
+      <c r="AO25" s="97"/>
+      <c r="AP25" s="97"/>
+      <c r="AQ25" s="97"/>
+      <c r="AR25" s="133"/>
+      <c r="AS25" s="133"/>
+      <c r="AT25" s="133"/>
+      <c r="AU25" s="133"/>
+      <c r="AV25" s="133"/>
+      <c r="AW25" s="133"/>
+      <c r="AX25" s="133"/>
     </row>
     <row r="26" spans="1:50" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="15">
         <v>2.06</v>
       </c>
-      <c r="C26" s="100" t="s">
-        <v>51</v>
+      <c r="C26" s="89" t="s">
+        <v>46</v>
       </c>
-      <c r="D26" s="100"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="38">
+      <c r="D26" s="89"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="36">
         <v>44535</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="18">
         <v>44535</v>
       </c>
-      <c r="H26" s="21" t="s">
-        <v>40</v>
+      <c r="H26" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I26" s="53" t="s">
+      <c r="I26" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="25"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="25"/>
-      <c r="AA26" s="25"/>
-      <c r="AB26" s="25"/>
-      <c r="AC26" s="25"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="25"/>
-      <c r="AG26" s="25"/>
-      <c r="AH26" s="25"/>
-      <c r="AI26" s="86"/>
-      <c r="AJ26" s="25"/>
-      <c r="AK26" s="31"/>
-      <c r="AL26" s="135"/>
-      <c r="AM26" s="135"/>
-      <c r="AN26" s="135"/>
-      <c r="AO26" s="135"/>
-      <c r="AP26" s="135"/>
-      <c r="AQ26" s="135"/>
-      <c r="AR26" s="95"/>
-      <c r="AS26" s="95"/>
-      <c r="AT26" s="95"/>
-      <c r="AU26" s="95"/>
-      <c r="AV26" s="95"/>
-      <c r="AW26" s="95"/>
-      <c r="AX26" s="95"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
+      <c r="AB26" s="23"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="23"/>
+      <c r="AG26" s="23"/>
+      <c r="AH26" s="23"/>
+      <c r="AI26" s="84"/>
+      <c r="AJ26" s="23"/>
+      <c r="AK26" s="29"/>
+      <c r="AL26" s="97"/>
+      <c r="AM26" s="97"/>
+      <c r="AN26" s="97"/>
+      <c r="AO26" s="97"/>
+      <c r="AP26" s="97"/>
+      <c r="AQ26" s="97"/>
+      <c r="AR26" s="133"/>
+      <c r="AS26" s="133"/>
+      <c r="AT26" s="133"/>
+      <c r="AU26" s="133"/>
+      <c r="AV26" s="133"/>
+      <c r="AW26" s="133"/>
+      <c r="AX26" s="133"/>
     </row>
     <row r="27" spans="1:50" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="15">
         <v>2.0699999999999998</v>
       </c>
-      <c r="C27" s="100" t="s">
-        <v>52</v>
+      <c r="C27" s="89" t="s">
+        <v>47</v>
       </c>
-      <c r="D27" s="100"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="38">
+      <c r="D27" s="89"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="36">
         <v>44535</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="18">
         <v>44535</v>
       </c>
-      <c r="H27" s="21" t="s">
-        <v>40</v>
+      <c r="H27" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I27" s="53" t="s">
+      <c r="I27" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="30"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="25"/>
-      <c r="AG27" s="25"/>
-      <c r="AH27" s="25"/>
-      <c r="AI27" s="86"/>
-      <c r="AJ27" s="25"/>
-      <c r="AK27" s="31"/>
-      <c r="AL27" s="135"/>
-      <c r="AM27" s="135"/>
-      <c r="AN27" s="135"/>
-      <c r="AO27" s="135"/>
-      <c r="AP27" s="135"/>
-      <c r="AQ27" s="135"/>
-      <c r="AR27" s="95"/>
-      <c r="AS27" s="95"/>
-      <c r="AT27" s="95"/>
-      <c r="AU27" s="95"/>
-      <c r="AV27" s="95"/>
-      <c r="AW27" s="95"/>
-      <c r="AX27" s="95"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="23"/>
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="23"/>
+      <c r="AI27" s="84"/>
+      <c r="AJ27" s="23"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="97"/>
+      <c r="AM27" s="97"/>
+      <c r="AN27" s="97"/>
+      <c r="AO27" s="97"/>
+      <c r="AP27" s="97"/>
+      <c r="AQ27" s="97"/>
+      <c r="AR27" s="133"/>
+      <c r="AS27" s="133"/>
+      <c r="AT27" s="133"/>
+      <c r="AU27" s="133"/>
+      <c r="AV27" s="133"/>
+      <c r="AW27" s="133"/>
+      <c r="AX27" s="133"/>
     </row>
     <row r="28" spans="1:50" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="15">
         <v>2.08</v>
       </c>
-      <c r="C28" s="100" t="s">
-        <v>56</v>
+      <c r="C28" s="89" t="s">
+        <v>51</v>
       </c>
-      <c r="D28" s="100"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="38">
+      <c r="D28" s="89"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="36">
         <v>44535</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="18">
         <v>44535</v>
       </c>
-      <c r="H28" s="21" t="s">
-        <v>40</v>
+      <c r="H28" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I28" s="53" t="s">
+      <c r="I28" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
-      <c r="AB28" s="25"/>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="31"/>
-      <c r="AE28" s="30"/>
-      <c r="AF28" s="25"/>
-      <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="86"/>
-      <c r="AJ28" s="25"/>
-      <c r="AK28" s="31"/>
-      <c r="AL28" s="135"/>
-      <c r="AM28" s="135"/>
-      <c r="AN28" s="135"/>
-      <c r="AO28" s="135"/>
-      <c r="AP28" s="135"/>
-      <c r="AQ28" s="135"/>
-      <c r="AR28" s="95"/>
-      <c r="AS28" s="95"/>
-      <c r="AT28" s="95"/>
-      <c r="AU28" s="95"/>
-      <c r="AV28" s="95"/>
-      <c r="AW28" s="95"/>
-      <c r="AX28" s="95"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="28"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="29"/>
+      <c r="AE28" s="28"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="23"/>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="84"/>
+      <c r="AJ28" s="23"/>
+      <c r="AK28" s="29"/>
+      <c r="AL28" s="97"/>
+      <c r="AM28" s="97"/>
+      <c r="AN28" s="97"/>
+      <c r="AO28" s="97"/>
+      <c r="AP28" s="97"/>
+      <c r="AQ28" s="97"/>
+      <c r="AR28" s="133"/>
+      <c r="AS28" s="133"/>
+      <c r="AT28" s="133"/>
+      <c r="AU28" s="133"/>
+      <c r="AV28" s="133"/>
+      <c r="AW28" s="133"/>
+      <c r="AX28" s="133"/>
     </row>
     <row r="29" spans="1:50" ht="14.25" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="15">
         <v>2.09</v>
       </c>
-      <c r="C29" s="100" t="s">
-        <v>54</v>
+      <c r="C29" s="89" t="s">
+        <v>49</v>
       </c>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="38">
+      <c r="D29" s="89"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="36">
         <v>44535</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="18">
         <v>44535</v>
       </c>
-      <c r="H29" s="21" t="s">
-        <v>40</v>
+      <c r="H29" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I29" s="53" t="s">
+      <c r="I29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="31"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25"/>
-      <c r="AD29" s="31"/>
-      <c r="AE29" s="30"/>
-      <c r="AF29" s="25"/>
-      <c r="AG29" s="25"/>
-      <c r="AH29" s="25"/>
-      <c r="AI29" s="86"/>
-      <c r="AJ29" s="25"/>
-      <c r="AK29" s="31"/>
-      <c r="AL29" s="135"/>
-      <c r="AM29" s="135"/>
-      <c r="AN29" s="135"/>
-      <c r="AO29" s="135"/>
-      <c r="AP29" s="135"/>
-      <c r="AQ29" s="135"/>
-      <c r="AR29" s="95"/>
-      <c r="AS29" s="95"/>
-      <c r="AT29" s="95"/>
-      <c r="AU29" s="95"/>
-      <c r="AV29" s="95"/>
-      <c r="AW29" s="95"/>
-      <c r="AX29" s="95"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="29"/>
+      <c r="AE29" s="28"/>
+      <c r="AF29" s="23"/>
+      <c r="AG29" s="23"/>
+      <c r="AH29" s="23"/>
+      <c r="AI29" s="84"/>
+      <c r="AJ29" s="23"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="97"/>
+      <c r="AM29" s="97"/>
+      <c r="AN29" s="97"/>
+      <c r="AO29" s="97"/>
+      <c r="AP29" s="97"/>
+      <c r="AQ29" s="97"/>
+      <c r="AR29" s="133"/>
+      <c r="AS29" s="133"/>
+      <c r="AT29" s="133"/>
+      <c r="AU29" s="133"/>
+      <c r="AV29" s="133"/>
+      <c r="AW29" s="133"/>
+      <c r="AX29" s="133"/>
     </row>
     <row r="30" spans="1:50" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="15">
         <v>2.1</v>
       </c>
-      <c r="C30" s="102" t="s">
-        <v>53</v>
+      <c r="C30" s="124" t="s">
+        <v>48</v>
       </c>
-      <c r="D30" s="102"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="38">
+      <c r="D30" s="124"/>
+      <c r="E30" s="125"/>
+      <c r="F30" s="36">
         <v>44535</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="18">
         <v>44536</v>
       </c>
-      <c r="H30" s="21" t="s">
-        <v>40</v>
+      <c r="H30" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="I30" s="53" t="s">
+      <c r="I30" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J30" s="30"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="25"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
-      <c r="AB30" s="25"/>
-      <c r="AC30" s="25"/>
-      <c r="AD30" s="31"/>
-      <c r="AE30" s="30"/>
-      <c r="AF30" s="25"/>
-      <c r="AG30" s="25"/>
-      <c r="AH30" s="25"/>
-      <c r="AI30" s="86"/>
-      <c r="AJ30" s="86"/>
-      <c r="AK30" s="31"/>
-      <c r="AL30" s="135"/>
-      <c r="AM30" s="135"/>
-      <c r="AN30" s="135"/>
-      <c r="AO30" s="135"/>
-      <c r="AP30" s="135"/>
-      <c r="AQ30" s="135"/>
-      <c r="AR30" s="95"/>
-      <c r="AS30" s="95"/>
-      <c r="AT30" s="95"/>
-      <c r="AU30" s="95"/>
-      <c r="AV30" s="95"/>
-      <c r="AW30" s="95"/>
-      <c r="AX30" s="95"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+      <c r="AA30" s="23"/>
+      <c r="AB30" s="23"/>
+      <c r="AC30" s="23"/>
+      <c r="AD30" s="29"/>
+      <c r="AE30" s="28"/>
+      <c r="AF30" s="23"/>
+      <c r="AG30" s="23"/>
+      <c r="AH30" s="23"/>
+      <c r="AI30" s="84"/>
+      <c r="AJ30" s="84"/>
+      <c r="AK30" s="29"/>
+      <c r="AL30" s="97"/>
+      <c r="AM30" s="97"/>
+      <c r="AN30" s="97"/>
+      <c r="AO30" s="97"/>
+      <c r="AP30" s="97"/>
+      <c r="AQ30" s="97"/>
+      <c r="AR30" s="133"/>
+      <c r="AS30" s="133"/>
+      <c r="AT30" s="133"/>
+      <c r="AU30" s="133"/>
+      <c r="AV30" s="133"/>
+      <c r="AW30" s="133"/>
+      <c r="AX30" s="133"/>
     </row>
     <row r="31" spans="1:50" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A31" s="10"/>
       <c r="B31" s="15">
         <v>2.11</v>
       </c>
-      <c r="C31" s="102" t="s">
-        <v>55</v>
+      <c r="C31" s="124" t="s">
+        <v>50</v>
       </c>
-      <c r="D31" s="102"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="38">
+      <c r="D31" s="124"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="36">
         <v>44536</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="18">
         <v>44536</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="54"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="30"/>
+      <c r="Z31" s="30"/>
+      <c r="AA31" s="30"/>
+      <c r="AB31" s="30"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="31"/>
+      <c r="AE31" s="56"/>
+      <c r="AF31" s="30"/>
+      <c r="AG31" s="30"/>
+      <c r="AH31" s="30"/>
+      <c r="AI31" s="87"/>
+      <c r="AJ31" s="87"/>
+      <c r="AK31" s="31"/>
+      <c r="AL31" s="97"/>
+      <c r="AM31" s="97"/>
+      <c r="AN31" s="97"/>
+      <c r="AO31" s="97"/>
+      <c r="AP31" s="97"/>
+      <c r="AQ31" s="97"/>
+      <c r="AR31" s="133"/>
+      <c r="AS31" s="133"/>
+      <c r="AT31" s="133"/>
+      <c r="AU31" s="133"/>
+      <c r="AV31" s="133"/>
+      <c r="AW31" s="133"/>
+      <c r="AX31" s="133"/>
+    </row>
+    <row r="32" spans="1:50" ht="14.25" customHeight="1">
+      <c r="A32" s="1"/>
+      <c r="B32" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="33"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="32"/>
-      <c r="AC31" s="32"/>
-      <c r="AD31" s="33"/>
-      <c r="AE31" s="58"/>
-      <c r="AF31" s="32"/>
-      <c r="AG31" s="32"/>
-      <c r="AH31" s="32"/>
-      <c r="AI31" s="89"/>
-      <c r="AJ31" s="89"/>
-      <c r="AK31" s="33"/>
-      <c r="AL31" s="135"/>
-      <c r="AM31" s="135"/>
-      <c r="AN31" s="135"/>
-      <c r="AO31" s="135"/>
-      <c r="AP31" s="135"/>
-      <c r="AQ31" s="135"/>
-      <c r="AR31" s="95"/>
-      <c r="AS31" s="95"/>
-      <c r="AT31" s="95"/>
-      <c r="AU31" s="95"/>
-      <c r="AV31" s="95"/>
-      <c r="AW31" s="95"/>
-      <c r="AX31" s="95"/>
-    </row>
-    <row r="32" spans="1:50" ht="14.25" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="104" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="65"/>
-      <c r="P32" s="66"/>
-      <c r="Q32" s="67"/>
-      <c r="R32" s="65"/>
-      <c r="S32" s="65"/>
-      <c r="T32" s="65"/>
-      <c r="U32" s="65"/>
-      <c r="V32" s="65"/>
-      <c r="W32" s="66"/>
-      <c r="X32" s="67"/>
-      <c r="Y32" s="65"/>
-      <c r="Z32" s="65"/>
-      <c r="AA32" s="65"/>
-      <c r="AB32" s="65"/>
-      <c r="AC32" s="65"/>
-      <c r="AD32" s="66"/>
-      <c r="AE32" s="67"/>
-      <c r="AF32" s="65"/>
-      <c r="AG32" s="65"/>
-      <c r="AH32" s="65"/>
-      <c r="AI32" s="65"/>
-      <c r="AJ32" s="65"/>
-      <c r="AK32" s="66"/>
-      <c r="AL32" s="135"/>
-      <c r="AM32" s="135"/>
-      <c r="AN32" s="135"/>
-      <c r="AO32" s="135"/>
-      <c r="AP32" s="135"/>
-      <c r="AQ32" s="135"/>
-      <c r="AR32" s="95"/>
-      <c r="AS32" s="95"/>
-      <c r="AT32" s="95"/>
-      <c r="AU32" s="95"/>
-      <c r="AV32" s="95"/>
-      <c r="AW32" s="95"/>
-      <c r="AX32" s="95"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="64"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="63"/>
+      <c r="Z32" s="63"/>
+      <c r="AA32" s="63"/>
+      <c r="AB32" s="63"/>
+      <c r="AC32" s="63"/>
+      <c r="AD32" s="64"/>
+      <c r="AE32" s="65"/>
+      <c r="AF32" s="63"/>
+      <c r="AG32" s="63"/>
+      <c r="AH32" s="63"/>
+      <c r="AI32" s="63"/>
+      <c r="AJ32" s="63"/>
+      <c r="AK32" s="64"/>
+      <c r="AL32" s="97"/>
+      <c r="AM32" s="97"/>
+      <c r="AN32" s="97"/>
+      <c r="AO32" s="97"/>
+      <c r="AP32" s="97"/>
+      <c r="AQ32" s="97"/>
+      <c r="AR32" s="133"/>
+      <c r="AS32" s="133"/>
+      <c r="AT32" s="133"/>
+      <c r="AU32" s="133"/>
+      <c r="AV32" s="133"/>
+      <c r="AW32" s="133"/>
+      <c r="AX32" s="133"/>
     </row>
     <row r="33" spans="1:50" ht="14.25" customHeight="1">
       <c r="A33" s="10"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="73"/>
-      <c r="Y33" s="74"/>
-      <c r="Z33" s="74"/>
-      <c r="AA33" s="74"/>
-      <c r="AB33" s="74"/>
-      <c r="AC33" s="74"/>
-      <c r="AD33" s="75"/>
-      <c r="AE33" s="73"/>
-      <c r="AF33" s="74"/>
-      <c r="AG33" s="74"/>
-      <c r="AH33" s="74"/>
-      <c r="AI33" s="74"/>
-      <c r="AJ33" s="74"/>
-      <c r="AK33" s="75"/>
-      <c r="AL33" s="135"/>
-      <c r="AM33" s="135"/>
-      <c r="AN33" s="135"/>
-      <c r="AO33" s="135"/>
-      <c r="AP33" s="135"/>
-      <c r="AQ33" s="135"/>
-      <c r="AR33" s="95"/>
-      <c r="AS33" s="95"/>
-      <c r="AT33" s="95"/>
-      <c r="AU33" s="95"/>
-      <c r="AV33" s="95"/>
-      <c r="AW33" s="95"/>
-      <c r="AX33" s="95"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72"/>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="72"/>
+      <c r="T33" s="72"/>
+      <c r="U33" s="72"/>
+      <c r="V33" s="72"/>
+      <c r="W33" s="73"/>
+      <c r="X33" s="71"/>
+      <c r="Y33" s="72"/>
+      <c r="Z33" s="72"/>
+      <c r="AA33" s="72"/>
+      <c r="AB33" s="72"/>
+      <c r="AC33" s="72"/>
+      <c r="AD33" s="73"/>
+      <c r="AE33" s="71"/>
+      <c r="AF33" s="72"/>
+      <c r="AG33" s="72"/>
+      <c r="AH33" s="72"/>
+      <c r="AI33" s="72"/>
+      <c r="AJ33" s="72"/>
+      <c r="AK33" s="73"/>
+      <c r="AL33" s="97"/>
+      <c r="AM33" s="97"/>
+      <c r="AN33" s="97"/>
+      <c r="AO33" s="97"/>
+      <c r="AP33" s="97"/>
+      <c r="AQ33" s="97"/>
+      <c r="AR33" s="133"/>
+      <c r="AS33" s="133"/>
+      <c r="AT33" s="133"/>
+      <c r="AU33" s="133"/>
+      <c r="AV33" s="133"/>
+      <c r="AW33" s="133"/>
+      <c r="AX33" s="133"/>
     </row>
     <row r="34" spans="1:50" ht="14.25" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="97"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="74"/>
-      <c r="O34" s="74"/>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="74"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="75"/>
-      <c r="X34" s="73"/>
-      <c r="Y34" s="74"/>
-      <c r="Z34" s="74"/>
-      <c r="AA34" s="74"/>
-      <c r="AB34" s="74"/>
-      <c r="AC34" s="74"/>
-      <c r="AD34" s="75"/>
-      <c r="AE34" s="73"/>
-      <c r="AF34" s="74"/>
-      <c r="AG34" s="74"/>
-      <c r="AH34" s="74"/>
-      <c r="AI34" s="74"/>
-      <c r="AJ34" s="74"/>
-      <c r="AK34" s="75"/>
-      <c r="AL34" s="135"/>
-      <c r="AM34" s="135"/>
-      <c r="AN34" s="135"/>
-      <c r="AO34" s="135"/>
-      <c r="AP34" s="135"/>
-      <c r="AQ34" s="135"/>
-      <c r="AR34" s="95"/>
-      <c r="AS34" s="95"/>
-      <c r="AT34" s="95"/>
-      <c r="AU34" s="95"/>
-      <c r="AV34" s="95"/>
-      <c r="AW34" s="95"/>
-      <c r="AX34" s="95"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="120"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="71"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="72"/>
+      <c r="T34" s="72"/>
+      <c r="U34" s="72"/>
+      <c r="V34" s="72"/>
+      <c r="W34" s="73"/>
+      <c r="X34" s="71"/>
+      <c r="Y34" s="72"/>
+      <c r="Z34" s="72"/>
+      <c r="AA34" s="72"/>
+      <c r="AB34" s="72"/>
+      <c r="AC34" s="72"/>
+      <c r="AD34" s="73"/>
+      <c r="AE34" s="71"/>
+      <c r="AF34" s="72"/>
+      <c r="AG34" s="72"/>
+      <c r="AH34" s="72"/>
+      <c r="AI34" s="72"/>
+      <c r="AJ34" s="72"/>
+      <c r="AK34" s="73"/>
+      <c r="AL34" s="97"/>
+      <c r="AM34" s="97"/>
+      <c r="AN34" s="97"/>
+      <c r="AO34" s="97"/>
+      <c r="AP34" s="97"/>
+      <c r="AQ34" s="97"/>
+      <c r="AR34" s="133"/>
+      <c r="AS34" s="133"/>
+      <c r="AT34" s="133"/>
+      <c r="AU34" s="133"/>
+      <c r="AV34" s="133"/>
+      <c r="AW34" s="133"/>
+      <c r="AX34" s="133"/>
     </row>
     <row r="35" spans="1:50" ht="14.25" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="75"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="74"/>
-      <c r="S35" s="74"/>
-      <c r="T35" s="74"/>
-      <c r="U35" s="74"/>
-      <c r="V35" s="74"/>
-      <c r="W35" s="75"/>
-      <c r="X35" s="73"/>
-      <c r="Y35" s="74"/>
-      <c r="Z35" s="74"/>
-      <c r="AA35" s="74"/>
-      <c r="AB35" s="74"/>
-      <c r="AC35" s="74"/>
-      <c r="AD35" s="75"/>
-      <c r="AE35" s="73"/>
-      <c r="AF35" s="74"/>
-      <c r="AG35" s="74"/>
-      <c r="AH35" s="74"/>
-      <c r="AI35" s="74"/>
-      <c r="AJ35" s="74"/>
-      <c r="AK35" s="75"/>
-      <c r="AL35" s="135"/>
-      <c r="AM35" s="135"/>
-      <c r="AN35" s="135"/>
-      <c r="AO35" s="135"/>
-      <c r="AP35" s="135"/>
-      <c r="AQ35" s="135"/>
-      <c r="AR35" s="95"/>
-      <c r="AS35" s="95"/>
-      <c r="AT35" s="95"/>
-      <c r="AU35" s="95"/>
-      <c r="AV35" s="95"/>
-      <c r="AW35" s="95"/>
-      <c r="AX35" s="95"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="72"/>
+      <c r="P35" s="73"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="73"/>
+      <c r="X35" s="71"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="72"/>
+      <c r="AA35" s="72"/>
+      <c r="AB35" s="72"/>
+      <c r="AC35" s="72"/>
+      <c r="AD35" s="73"/>
+      <c r="AE35" s="71"/>
+      <c r="AF35" s="72"/>
+      <c r="AG35" s="72"/>
+      <c r="AH35" s="72"/>
+      <c r="AI35" s="72"/>
+      <c r="AJ35" s="72"/>
+      <c r="AK35" s="73"/>
+      <c r="AL35" s="97"/>
+      <c r="AM35" s="97"/>
+      <c r="AN35" s="97"/>
+      <c r="AO35" s="97"/>
+      <c r="AP35" s="97"/>
+      <c r="AQ35" s="97"/>
+      <c r="AR35" s="133"/>
+      <c r="AS35" s="133"/>
+      <c r="AT35" s="133"/>
+      <c r="AU35" s="133"/>
+      <c r="AV35" s="133"/>
+      <c r="AW35" s="133"/>
+      <c r="AX35" s="133"/>
     </row>
     <row r="36" spans="1:50" ht="14.25" customHeight="1" thickBot="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="84"/>
-      <c r="L36" s="84"/>
-      <c r="M36" s="84"/>
-      <c r="N36" s="84"/>
-      <c r="O36" s="84"/>
-      <c r="P36" s="85"/>
-      <c r="Q36" s="83"/>
-      <c r="R36" s="84"/>
-      <c r="S36" s="84"/>
-      <c r="T36" s="84"/>
-      <c r="U36" s="84"/>
-      <c r="V36" s="84"/>
-      <c r="W36" s="85"/>
-      <c r="X36" s="83"/>
-      <c r="Y36" s="84"/>
-      <c r="Z36" s="84"/>
-      <c r="AA36" s="84"/>
-      <c r="AB36" s="84"/>
-      <c r="AC36" s="84"/>
-      <c r="AD36" s="85"/>
-      <c r="AE36" s="83"/>
-      <c r="AF36" s="84"/>
-      <c r="AG36" s="84"/>
-      <c r="AH36" s="84"/>
-      <c r="AI36" s="84"/>
-      <c r="AJ36" s="84"/>
-      <c r="AK36" s="85"/>
-      <c r="AL36" s="135"/>
-      <c r="AM36" s="135"/>
-      <c r="AN36" s="135"/>
-      <c r="AO36" s="135"/>
-      <c r="AP36" s="135"/>
-      <c r="AQ36" s="135"/>
-      <c r="AR36" s="95"/>
-      <c r="AS36" s="95"/>
-      <c r="AT36" s="95"/>
-      <c r="AU36" s="95"/>
-      <c r="AV36" s="95"/>
-      <c r="AW36" s="95"/>
-      <c r="AX36" s="95"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="82"/>
+      <c r="P36" s="83"/>
+      <c r="Q36" s="81"/>
+      <c r="R36" s="82"/>
+      <c r="S36" s="82"/>
+      <c r="T36" s="82"/>
+      <c r="U36" s="82"/>
+      <c r="V36" s="82"/>
+      <c r="W36" s="83"/>
+      <c r="X36" s="81"/>
+      <c r="Y36" s="82"/>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="82"/>
+      <c r="AB36" s="82"/>
+      <c r="AC36" s="82"/>
+      <c r="AD36" s="83"/>
+      <c r="AE36" s="81"/>
+      <c r="AF36" s="82"/>
+      <c r="AG36" s="82"/>
+      <c r="AH36" s="82"/>
+      <c r="AI36" s="82"/>
+      <c r="AJ36" s="82"/>
+      <c r="AK36" s="83"/>
+      <c r="AL36" s="97"/>
+      <c r="AM36" s="97"/>
+      <c r="AN36" s="97"/>
+      <c r="AO36" s="97"/>
+      <c r="AP36" s="97"/>
+      <c r="AQ36" s="97"/>
+      <c r="AR36" s="133"/>
+      <c r="AS36" s="133"/>
+      <c r="AT36" s="133"/>
+      <c r="AU36" s="133"/>
+      <c r="AV36" s="133"/>
+      <c r="AW36" s="133"/>
+      <c r="AX36" s="133"/>
     </row>
     <row r="37" spans="1:50" ht="14.25" customHeight="1">
       <c r="A37" s="1"/>
@@ -53110,26 +53120,12 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="AL11:AQ36"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B11:E13"/>
+    <mergeCell ref="K10:Z10"/>
+    <mergeCell ref="AE11:AK11"/>
+    <mergeCell ref="Q11:W11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="AR11:AX36"/>
+    <mergeCell ref="X11:AD11"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C22:E22"/>
@@ -53141,12 +53137,26 @@
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
-    <mergeCell ref="K10:Z10"/>
-    <mergeCell ref="AE11:AK11"/>
-    <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="AR11:AX36"/>
-    <mergeCell ref="X11:AD11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="AL11:AQ36"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
Update related to Sprint 2, from Phase 2
</commit_message>
<xml_diff>
--- a/project/Work breakdown structure.xlsx
+++ b/project/Work breakdown structure.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao4\IdeaProjects\SE2122-57672-58175-57957-58210-57911\project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C826C7-72B7-4858-84F5-0CBDBB03B21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
   <si>
     <t>Done</t>
   </si>
@@ -347,11 +341,32 @@
   <si>
     <t>58175+57911</t>
   </si>
+  <si>
+    <t>Implementation phase</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>Implement functionality 1 fully</t>
+  </si>
+  <si>
+    <t>Implement functionality 2 fully</t>
+  </si>
+  <si>
+    <t>Christmas Break</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
@@ -426,6 +441,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -526,7 +542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1069,11 +1085,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1365,59 +1405,29 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1485,23 +1495,93 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1717,15 +1797,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO1066"/>
+  <dimension ref="A1:BO1070"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BB40" sqref="BB40"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BE10" sqref="BE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -1734,7 +1814,7 @@
     <col min="2" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="50.25" customWidth="1"/>
     <col min="6" max="7" width="10.75" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="18.125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="18.08203125" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="10.75" customWidth="1" outlineLevel="1"/>
     <col min="10" max="30" width="6" style="12" customWidth="1"/>
     <col min="31" max="32" width="6" customWidth="1"/>
@@ -1744,13 +1824,13 @@
     <col min="52" max="52" width="6" customWidth="1"/>
     <col min="53" max="54" width="6.25" customWidth="1"/>
     <col min="55" max="55" width="6" customWidth="1"/>
-    <col min="56" max="56" width="5.875" customWidth="1"/>
+    <col min="56" max="56" width="5.83203125" customWidth="1"/>
     <col min="57" max="58" width="6" customWidth="1"/>
-    <col min="59" max="60" width="5.875" customWidth="1"/>
+    <col min="59" max="60" width="5.83203125" customWidth="1"/>
     <col min="61" max="61" width="6.25" customWidth="1"/>
-    <col min="62" max="62" width="6.375" customWidth="1"/>
+    <col min="62" max="62" width="6.33203125" customWidth="1"/>
     <col min="63" max="63" width="6" customWidth="1"/>
-    <col min="64" max="64" width="6.125" customWidth="1"/>
+    <col min="64" max="64" width="6.08203125" customWidth="1"/>
     <col min="65" max="65" width="6" customWidth="1"/>
     <col min="66" max="66" width="4.5" customWidth="1"/>
   </cols>
@@ -1826,12 +1906,12 @@
     </row>
     <row r="2" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
@@ -2110,10 +2190,10 @@
     </row>
     <row r="6" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="124"/>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
+      <c r="B6" s="114"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
@@ -2186,7 +2266,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="13">
         <f ca="1">TODAY()</f>
-        <v>44557</v>
+        <v>44559</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2408,24 +2488,24 @@
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="103" t="s">
+      <c r="K10" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="103"/>
-      <c r="Q10" s="103"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="103"/>
-      <c r="T10" s="103"/>
-      <c r="U10" s="103"/>
-      <c r="V10" s="103"/>
-      <c r="W10" s="103"/>
-      <c r="X10" s="103"/>
-      <c r="Y10" s="103"/>
-      <c r="Z10" s="103"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="142"/>
+      <c r="S10" s="142"/>
+      <c r="T10" s="142"/>
+      <c r="U10" s="142"/>
+      <c r="V10" s="142"/>
+      <c r="W10" s="142"/>
+      <c r="X10" s="142"/>
+      <c r="Y10" s="142"/>
+      <c r="Z10" s="142"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -2453,8 +2533,10 @@
       <c r="AY10" s="96"/>
       <c r="AZ10" s="96"/>
       <c r="BA10" s="96"/>
-      <c r="BB10" s="96"/>
-      <c r="BC10" s="96"/>
+      <c r="BB10" s="142" t="s">
+        <v>110</v>
+      </c>
+      <c r="BC10" s="142"/>
       <c r="BD10" s="96"/>
       <c r="BE10" s="96"/>
       <c r="BF10" s="96"/>
@@ -2470,109 +2552,109 @@
     </row>
     <row r="11" spans="1:67" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="137" t="s">
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="137" t="s">
+      <c r="G11" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="137" t="s">
+      <c r="H11" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="140" t="s">
+      <c r="I11" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="98"/>
-      <c r="O11" s="98"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="97" t="s">
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+      <c r="O11" s="137"/>
+      <c r="P11" s="138"/>
+      <c r="Q11" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="98"/>
-      <c r="S11" s="98"/>
-      <c r="T11" s="98"/>
-      <c r="U11" s="98"/>
-      <c r="V11" s="98"/>
-      <c r="W11" s="99"/>
-      <c r="X11" s="97" t="s">
+      <c r="R11" s="137"/>
+      <c r="S11" s="137"/>
+      <c r="T11" s="137"/>
+      <c r="U11" s="137"/>
+      <c r="V11" s="137"/>
+      <c r="W11" s="138"/>
+      <c r="X11" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="Y11" s="98"/>
-      <c r="Z11" s="98"/>
-      <c r="AA11" s="98"/>
-      <c r="AB11" s="98"/>
-      <c r="AC11" s="98"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="97" t="s">
+      <c r="Y11" s="137"/>
+      <c r="Z11" s="137"/>
+      <c r="AA11" s="137"/>
+      <c r="AB11" s="137"/>
+      <c r="AC11" s="137"/>
+      <c r="AD11" s="138"/>
+      <c r="AE11" s="136" t="s">
         <v>13</v>
       </c>
-      <c r="AF11" s="98"/>
-      <c r="AG11" s="98"/>
-      <c r="AH11" s="98"/>
-      <c r="AI11" s="98"/>
-      <c r="AJ11" s="98"/>
-      <c r="AK11" s="99"/>
-      <c r="AL11" s="97" t="s">
+      <c r="AF11" s="137"/>
+      <c r="AG11" s="137"/>
+      <c r="AH11" s="137"/>
+      <c r="AI11" s="137"/>
+      <c r="AJ11" s="137"/>
+      <c r="AK11" s="138"/>
+      <c r="AL11" s="136" t="s">
         <v>70</v>
       </c>
-      <c r="AM11" s="98"/>
-      <c r="AN11" s="98"/>
-      <c r="AO11" s="98"/>
-      <c r="AP11" s="98"/>
-      <c r="AQ11" s="98"/>
-      <c r="AR11" s="99"/>
-      <c r="AS11" s="97" t="s">
+      <c r="AM11" s="137"/>
+      <c r="AN11" s="137"/>
+      <c r="AO11" s="137"/>
+      <c r="AP11" s="137"/>
+      <c r="AQ11" s="137"/>
+      <c r="AR11" s="138"/>
+      <c r="AS11" s="136" t="s">
         <v>92</v>
       </c>
-      <c r="AT11" s="98"/>
-      <c r="AU11" s="98"/>
-      <c r="AV11" s="98"/>
-      <c r="AW11" s="98"/>
-      <c r="AX11" s="98"/>
-      <c r="AY11" s="99"/>
-      <c r="AZ11" s="97" t="s">
+      <c r="AT11" s="137"/>
+      <c r="AU11" s="137"/>
+      <c r="AV11" s="137"/>
+      <c r="AW11" s="137"/>
+      <c r="AX11" s="137"/>
+      <c r="AY11" s="138"/>
+      <c r="AZ11" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="BA11" s="98"/>
-      <c r="BB11" s="98"/>
-      <c r="BC11" s="98"/>
-      <c r="BD11" s="98"/>
-      <c r="BE11" s="98"/>
-      <c r="BF11" s="99"/>
-      <c r="BG11" s="100" t="s">
+      <c r="BA11" s="137"/>
+      <c r="BB11" s="137"/>
+      <c r="BC11" s="137"/>
+      <c r="BD11" s="137"/>
+      <c r="BE11" s="137"/>
+      <c r="BF11" s="138"/>
+      <c r="BG11" s="139" t="s">
         <v>94</v>
       </c>
-      <c r="BH11" s="101"/>
-      <c r="BI11" s="101"/>
-      <c r="BJ11" s="101"/>
-      <c r="BK11" s="101"/>
-      <c r="BL11" s="101"/>
-      <c r="BM11" s="102"/>
+      <c r="BH11" s="140"/>
+      <c r="BI11" s="140"/>
+      <c r="BJ11" s="140"/>
+      <c r="BK11" s="140"/>
+      <c r="BL11" s="140"/>
+      <c r="BM11" s="141"/>
       <c r="BN11" s="96"/>
       <c r="BO11" s="96"/>
     </row>
     <row r="12" spans="1:67" ht="14.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="141"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="101"/>
       <c r="J12" s="24" t="s">
         <v>14</v>
       </c>
@@ -2746,14 +2828,14 @@
     </row>
     <row r="13" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="135"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="139"/>
-      <c r="G13" s="139"/>
-      <c r="H13" s="139"/>
-      <c r="I13" s="142"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="102"/>
       <c r="J13" s="26">
         <v>44510</v>
       </c>
@@ -2927,12 +3009,12 @@
     </row>
     <row r="14" spans="1:67" ht="16.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -3003,11 +3085,11 @@
       <c r="B15" s="61">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="116"/>
       <c r="F15" s="20">
         <v>44510</v>
       </c>
@@ -3084,11 +3166,11 @@
       <c r="B16" s="61">
         <v>1.2</v>
       </c>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="126"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="116"/>
       <c r="F16" s="20">
         <v>44510</v>
       </c>
@@ -3165,11 +3247,11 @@
       <c r="B17" s="61">
         <v>1.3</v>
       </c>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="126"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="116"/>
       <c r="F17" s="21">
         <v>44535</v>
       </c>
@@ -3246,11 +3328,11 @@
       <c r="B18" s="61">
         <v>1.4</v>
       </c>
-      <c r="C18" s="109" t="s">
+      <c r="C18" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="125"/>
-      <c r="E18" s="126"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="116"/>
       <c r="F18" s="21">
         <v>44535</v>
       </c>
@@ -3327,11 +3409,11 @@
       <c r="B19" s="62">
         <v>1.5</v>
       </c>
-      <c r="C19" s="127" t="s">
+      <c r="C19" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="129"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="119"/>
       <c r="F19" s="21">
         <v>44535</v>
       </c>
@@ -3405,12 +3487,12 @@
     </row>
     <row r="20" spans="1:67" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="10"/>
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="123"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="41"/>
       <c r="G20" s="33"/>
       <c r="H20" s="34"/>
@@ -3479,11 +3561,11 @@
       <c r="B21" s="15">
         <v>2.0099999999999998</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="109"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="104"/>
       <c r="F21" s="36">
         <v>44527</v>
       </c>
@@ -3560,11 +3642,11 @@
       <c r="B22" s="15">
         <v>2.02</v>
       </c>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="108"/>
-      <c r="E22" s="109"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="104"/>
       <c r="F22" s="36">
         <v>44527</v>
       </c>
@@ -3641,11 +3723,11 @@
       <c r="B23" s="15">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="108"/>
-      <c r="E23" s="109"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="104"/>
       <c r="F23" s="36">
         <v>44533</v>
       </c>
@@ -3722,11 +3804,11 @@
       <c r="B24" s="15">
         <v>2.04</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="109"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="104"/>
       <c r="F24" s="36">
         <v>44533</v>
       </c>
@@ -3803,11 +3885,11 @@
       <c r="B25" s="15">
         <v>2.0499999999999998</v>
       </c>
-      <c r="C25" s="108" t="s">
+      <c r="C25" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="104"/>
       <c r="F25" s="36">
         <v>44533</v>
       </c>
@@ -3884,11 +3966,11 @@
       <c r="B26" s="15">
         <v>2.06</v>
       </c>
-      <c r="C26" s="108" t="s">
+      <c r="C26" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="108"/>
-      <c r="E26" s="109"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="104"/>
       <c r="F26" s="36">
         <v>44535</v>
       </c>
@@ -3965,11 +4047,11 @@
       <c r="B27" s="15">
         <v>2.0699999999999998</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="108"/>
-      <c r="E27" s="109"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="104"/>
       <c r="F27" s="36">
         <v>44535</v>
       </c>
@@ -4046,11 +4128,11 @@
       <c r="B28" s="15">
         <v>2.08</v>
       </c>
-      <c r="C28" s="108" t="s">
+      <c r="C28" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="109"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="104"/>
       <c r="F28" s="36">
         <v>44535</v>
       </c>
@@ -4127,11 +4209,11 @@
       <c r="B29" s="15">
         <v>2.09</v>
       </c>
-      <c r="C29" s="108" t="s">
+      <c r="C29" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="109"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="104"/>
       <c r="F29" s="36">
         <v>44535</v>
       </c>
@@ -4208,11 +4290,11 @@
       <c r="B30" s="15">
         <v>2.1</v>
       </c>
-      <c r="C30" s="110" t="s">
+      <c r="C30" s="131" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="110"/>
-      <c r="E30" s="111"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
       <c r="F30" s="36">
         <v>44535</v>
       </c>
@@ -4286,14 +4368,14 @@
     </row>
     <row r="31" spans="1:67" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A31" s="10"/>
-      <c r="B31" s="15">
-        <v>2.11</v>
+      <c r="B31" s="155" t="s">
+        <v>105</v>
       </c>
-      <c r="C31" s="110" t="s">
+      <c r="C31" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="110"/>
-      <c r="E31" s="111"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
       <c r="F31" s="36">
         <v>44536</v>
       </c>
@@ -4367,12 +4449,12 @@
     </row>
     <row r="32" spans="1:67" ht="14.25" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="112" t="s">
+      <c r="B32" s="133" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="114"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="135"/>
       <c r="F32" s="41"/>
       <c r="G32" s="33"/>
       <c r="H32" s="34"/>
@@ -4441,11 +4523,11 @@
       <c r="B33" s="63">
         <v>3.01</v>
       </c>
-      <c r="C33" s="104" t="s">
+      <c r="C33" s="127" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="105"/>
-      <c r="E33" s="105"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
       <c r="F33" s="64">
         <v>44545</v>
       </c>
@@ -4522,11 +4604,11 @@
       <c r="B34" s="63">
         <v>3.02</v>
       </c>
-      <c r="C34" s="104" t="s">
+      <c r="C34" s="127" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
       <c r="F34" s="64">
         <v>44545</v>
       </c>
@@ -4603,11 +4685,11 @@
       <c r="B35" s="63">
         <v>3.03</v>
       </c>
-      <c r="C35" s="104" t="s">
+      <c r="C35" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
       <c r="F35" s="64">
         <v>44545</v>
       </c>
@@ -4679,355 +4761,371 @@
       <c r="BN35" s="96"/>
       <c r="BO35" s="96"/>
     </row>
-    <row r="36" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="75"/>
-      <c r="L36" s="75"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="75"/>
-      <c r="O36" s="75"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="70"/>
-      <c r="R36" s="75"/>
-      <c r="S36" s="75"/>
-      <c r="T36" s="75"/>
-      <c r="U36" s="75"/>
-      <c r="V36" s="75"/>
-      <c r="W36" s="76"/>
-      <c r="X36" s="70"/>
-      <c r="Y36" s="75"/>
-      <c r="Z36" s="75"/>
-      <c r="AA36" s="75"/>
-      <c r="AB36" s="75"/>
-      <c r="AC36" s="75"/>
-      <c r="AD36" s="76"/>
-      <c r="AE36" s="70"/>
-      <c r="AF36" s="75"/>
-      <c r="AG36" s="75"/>
-      <c r="AH36" s="75"/>
-      <c r="AI36" s="75"/>
-      <c r="AJ36" s="75"/>
-      <c r="AK36" s="76"/>
-      <c r="AL36" s="70"/>
-      <c r="AM36" s="75"/>
-      <c r="AN36" s="75"/>
-      <c r="AO36" s="75"/>
-      <c r="AP36" s="75"/>
-      <c r="AQ36" s="75"/>
-      <c r="AR36" s="76"/>
-      <c r="AS36" s="70"/>
-      <c r="AT36" s="75"/>
-      <c r="AU36" s="75"/>
-      <c r="AV36" s="75"/>
-      <c r="AW36" s="75"/>
-      <c r="AX36" s="75"/>
-      <c r="AY36" s="76"/>
-      <c r="AZ36" s="70"/>
-      <c r="BA36" s="75"/>
-      <c r="BB36" s="75"/>
-      <c r="BC36" s="75"/>
-      <c r="BD36" s="75"/>
-      <c r="BE36" s="75"/>
-      <c r="BF36" s="76"/>
-      <c r="BG36" s="70"/>
-      <c r="BH36" s="75"/>
-      <c r="BI36" s="87"/>
-      <c r="BJ36" s="87"/>
-      <c r="BK36" s="87"/>
-      <c r="BL36" s="87"/>
-      <c r="BM36" s="88"/>
+    <row r="36" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="143">
+        <v>3.1</v>
+      </c>
+      <c r="C36" s="154" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="128"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="144"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="146"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="152"/>
+      <c r="K36" s="147"/>
+      <c r="L36" s="147"/>
+      <c r="M36" s="147"/>
+      <c r="N36" s="147"/>
+      <c r="O36" s="147"/>
+      <c r="P36" s="148"/>
+      <c r="Q36" s="143"/>
+      <c r="R36" s="147"/>
+      <c r="S36" s="147"/>
+      <c r="T36" s="147"/>
+      <c r="U36" s="147"/>
+      <c r="V36" s="147"/>
+      <c r="W36" s="148"/>
+      <c r="X36" s="143"/>
+      <c r="Y36" s="147"/>
+      <c r="Z36" s="147"/>
+      <c r="AA36" s="147"/>
+      <c r="AB36" s="147"/>
+      <c r="AC36" s="147"/>
+      <c r="AD36" s="148"/>
+      <c r="AE36" s="143"/>
+      <c r="AF36" s="147"/>
+      <c r="AG36" s="147"/>
+      <c r="AH36" s="147"/>
+      <c r="AI36" s="147"/>
+      <c r="AJ36" s="147"/>
+      <c r="AK36" s="148"/>
+      <c r="AL36" s="143"/>
+      <c r="AM36" s="147"/>
+      <c r="AN36" s="147"/>
+      <c r="AO36" s="147"/>
+      <c r="AP36" s="147"/>
+      <c r="AQ36" s="147"/>
+      <c r="AR36" s="148"/>
+      <c r="AS36" s="143"/>
+      <c r="AT36" s="147"/>
+      <c r="AU36" s="147"/>
+      <c r="AV36" s="147"/>
+      <c r="AW36" s="147"/>
+      <c r="AX36" s="147"/>
+      <c r="AY36" s="148"/>
+      <c r="AZ36" s="143"/>
+      <c r="BA36" s="147"/>
+      <c r="BB36" s="147"/>
+      <c r="BC36" s="147"/>
+      <c r="BD36" s="147"/>
+      <c r="BE36" s="147"/>
+      <c r="BF36" s="148"/>
+      <c r="BG36" s="143"/>
+      <c r="BH36" s="147"/>
+      <c r="BI36" s="149"/>
+      <c r="BJ36" s="149"/>
+      <c r="BK36" s="149"/>
+      <c r="BL36" s="149"/>
+      <c r="BM36" s="150"/>
       <c r="BN36" s="96"/>
       <c r="BO36" s="96"/>
     </row>
-    <row r="37" spans="1:67" ht="14.25" customHeight="1">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-      <c r="AF37" s="1"/>
-      <c r="AG37" s="1"/>
-      <c r="AH37" s="1"/>
-      <c r="AI37" s="1"/>
-      <c r="AJ37" s="1"/>
-      <c r="AK37" s="1"/>
-      <c r="AL37" s="1"/>
-      <c r="AM37" s="1"/>
-      <c r="AN37" s="1"/>
-      <c r="AO37" s="1"/>
-      <c r="AP37" s="1"/>
-      <c r="AQ37" s="1"/>
-      <c r="AR37" s="1"/>
-      <c r="AS37" s="1"/>
-      <c r="AT37" s="1"/>
-      <c r="AU37" s="1"/>
-      <c r="AV37" s="1"/>
-      <c r="AW37" s="1"/>
-      <c r="AX37" s="3"/>
-      <c r="AY37" s="96"/>
-      <c r="AZ37" s="96"/>
-      <c r="BA37" s="96"/>
-      <c r="BB37" s="96"/>
-      <c r="BC37" s="96"/>
-      <c r="BD37" s="96"/>
-      <c r="BE37" s="96"/>
-      <c r="BF37" s="96"/>
-      <c r="BG37" s="96"/>
-      <c r="BH37" s="96"/>
-      <c r="BI37" s="96"/>
-      <c r="BJ37" s="96"/>
-      <c r="BK37" s="96"/>
-      <c r="BL37" s="96"/>
-      <c r="BM37" s="96"/>
+    <row r="37" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A37" s="10"/>
+      <c r="B37" s="156" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="154" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="128"/>
+      <c r="E37" s="151"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="145"/>
+      <c r="H37" s="146"/>
+      <c r="I37" s="153" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="152"/>
+      <c r="K37" s="147"/>
+      <c r="L37" s="147"/>
+      <c r="M37" s="147"/>
+      <c r="N37" s="147"/>
+      <c r="O37" s="147"/>
+      <c r="P37" s="148"/>
+      <c r="Q37" s="143"/>
+      <c r="R37" s="147"/>
+      <c r="S37" s="147"/>
+      <c r="T37" s="147"/>
+      <c r="U37" s="147"/>
+      <c r="V37" s="147"/>
+      <c r="W37" s="148"/>
+      <c r="X37" s="143"/>
+      <c r="Y37" s="147"/>
+      <c r="Z37" s="147"/>
+      <c r="AA37" s="147"/>
+      <c r="AB37" s="147"/>
+      <c r="AC37" s="147"/>
+      <c r="AD37" s="148"/>
+      <c r="AE37" s="143"/>
+      <c r="AF37" s="147"/>
+      <c r="AG37" s="147"/>
+      <c r="AH37" s="147"/>
+      <c r="AI37" s="147"/>
+      <c r="AJ37" s="147"/>
+      <c r="AK37" s="148"/>
+      <c r="AL37" s="143"/>
+      <c r="AM37" s="147"/>
+      <c r="AN37" s="147"/>
+      <c r="AO37" s="147"/>
+      <c r="AP37" s="147"/>
+      <c r="AQ37" s="147"/>
+      <c r="AR37" s="148"/>
+      <c r="AS37" s="143"/>
+      <c r="AT37" s="147"/>
+      <c r="AU37" s="147"/>
+      <c r="AV37" s="147"/>
+      <c r="AW37" s="147"/>
+      <c r="AX37" s="147"/>
+      <c r="AY37" s="148"/>
+      <c r="AZ37" s="143"/>
+      <c r="BA37" s="147"/>
+      <c r="BB37" s="147"/>
+      <c r="BC37" s="147"/>
+      <c r="BD37" s="94"/>
+      <c r="BE37" s="94"/>
+      <c r="BF37" s="94"/>
+      <c r="BG37" s="94"/>
+      <c r="BH37" s="147"/>
+      <c r="BI37" s="149"/>
+      <c r="BJ37" s="149"/>
+      <c r="BK37" s="149"/>
+      <c r="BL37" s="149"/>
+      <c r="BM37" s="150"/>
       <c r="BN37" s="96"/>
       <c r="BO37" s="96"/>
     </row>
-    <row r="38" spans="1:67" ht="14.25" customHeight="1">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-      <c r="AG38" s="1"/>
-      <c r="AH38" s="1"/>
-      <c r="AI38" s="1"/>
-      <c r="AJ38" s="1"/>
-      <c r="AK38" s="1"/>
-      <c r="AL38" s="1"/>
-      <c r="AM38" s="1"/>
-      <c r="AN38" s="1"/>
-      <c r="AO38" s="1"/>
-      <c r="AP38" s="1"/>
-      <c r="AQ38" s="1"/>
-      <c r="AR38" s="1"/>
-      <c r="AS38" s="1"/>
-      <c r="AT38" s="1"/>
-      <c r="AU38" s="1"/>
-      <c r="AV38" s="1"/>
-      <c r="AW38" s="1"/>
-      <c r="AX38" s="3"/>
-      <c r="AY38" s="96"/>
-      <c r="AZ38" s="96"/>
-      <c r="BA38" s="96"/>
-      <c r="BB38" s="96"/>
-      <c r="BC38" s="96"/>
-      <c r="BD38" s="96"/>
-      <c r="BE38" s="96"/>
-      <c r="BF38" s="96"/>
-      <c r="BG38" s="96"/>
-      <c r="BH38" s="96"/>
-      <c r="BI38" s="96"/>
-      <c r="BJ38" s="96"/>
-      <c r="BK38" s="96"/>
-      <c r="BL38" s="96"/>
-      <c r="BM38" s="96"/>
+    <row r="38" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A38" s="10"/>
+      <c r="B38" s="156" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="154" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="128"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="146"/>
+      <c r="I38" s="153" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="152"/>
+      <c r="K38" s="147"/>
+      <c r="L38" s="147"/>
+      <c r="M38" s="147"/>
+      <c r="N38" s="147"/>
+      <c r="O38" s="147"/>
+      <c r="P38" s="148"/>
+      <c r="Q38" s="143"/>
+      <c r="R38" s="147"/>
+      <c r="S38" s="147"/>
+      <c r="T38" s="147"/>
+      <c r="U38" s="147"/>
+      <c r="V38" s="147"/>
+      <c r="W38" s="148"/>
+      <c r="X38" s="143"/>
+      <c r="Y38" s="147"/>
+      <c r="Z38" s="147"/>
+      <c r="AA38" s="147"/>
+      <c r="AB38" s="147"/>
+      <c r="AC38" s="147"/>
+      <c r="AD38" s="148"/>
+      <c r="AE38" s="143"/>
+      <c r="AF38" s="147"/>
+      <c r="AG38" s="147"/>
+      <c r="AH38" s="147"/>
+      <c r="AI38" s="147"/>
+      <c r="AJ38" s="147"/>
+      <c r="AK38" s="148"/>
+      <c r="AL38" s="143"/>
+      <c r="AM38" s="147"/>
+      <c r="AN38" s="147"/>
+      <c r="AO38" s="147"/>
+      <c r="AP38" s="147"/>
+      <c r="AQ38" s="147"/>
+      <c r="AR38" s="148"/>
+      <c r="AS38" s="143"/>
+      <c r="AT38" s="147"/>
+      <c r="AU38" s="147"/>
+      <c r="AV38" s="147"/>
+      <c r="AW38" s="147"/>
+      <c r="AX38" s="147"/>
+      <c r="AY38" s="148"/>
+      <c r="AZ38" s="143"/>
+      <c r="BA38" s="147"/>
+      <c r="BB38" s="147"/>
+      <c r="BC38" s="147"/>
+      <c r="BD38" s="94"/>
+      <c r="BE38" s="94"/>
+      <c r="BF38" s="94"/>
+      <c r="BG38" s="94"/>
+      <c r="BH38" s="147"/>
+      <c r="BI38" s="149"/>
+      <c r="BJ38" s="149"/>
+      <c r="BK38" s="149"/>
+      <c r="BL38" s="149"/>
+      <c r="BM38" s="150"/>
       <c r="BN38" s="96"/>
       <c r="BO38" s="96"/>
     </row>
-    <row r="39" spans="1:67" ht="16.5" customHeight="1">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-      <c r="AG39" s="1"/>
-      <c r="AH39" s="1"/>
-      <c r="AI39" s="1"/>
-      <c r="AJ39" s="1"/>
-      <c r="AK39" s="1"/>
-      <c r="AL39" s="1"/>
-      <c r="AM39" s="1"/>
-      <c r="AN39" s="1"/>
-      <c r="AO39" s="1"/>
-      <c r="AP39" s="1"/>
-      <c r="AQ39" s="1"/>
-      <c r="AR39" s="1"/>
-      <c r="AS39" s="1"/>
-      <c r="AT39" s="1"/>
-      <c r="AU39" s="1"/>
-      <c r="AV39" s="1"/>
-      <c r="AW39" s="1"/>
-      <c r="AX39" s="3"/>
-      <c r="AY39" s="96"/>
-      <c r="AZ39" s="96"/>
-      <c r="BA39" s="96"/>
-      <c r="BB39" s="96"/>
-      <c r="BC39" s="96"/>
-      <c r="BD39" s="96"/>
-      <c r="BE39" s="96"/>
-      <c r="BF39" s="96"/>
-      <c r="BG39" s="96"/>
-      <c r="BH39" s="96"/>
-      <c r="BI39" s="96"/>
-      <c r="BJ39" s="96"/>
-      <c r="BK39" s="96"/>
-      <c r="BL39" s="96"/>
-      <c r="BM39" s="96"/>
+    <row r="39" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="156"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="151"/>
+      <c r="F39" s="144"/>
+      <c r="G39" s="145"/>
+      <c r="H39" s="146"/>
+      <c r="I39" s="153"/>
+      <c r="J39" s="152"/>
+      <c r="K39" s="147"/>
+      <c r="L39" s="147"/>
+      <c r="M39" s="147"/>
+      <c r="N39" s="147"/>
+      <c r="O39" s="147"/>
+      <c r="P39" s="148"/>
+      <c r="Q39" s="143"/>
+      <c r="R39" s="147"/>
+      <c r="S39" s="147"/>
+      <c r="T39" s="147"/>
+      <c r="U39" s="147"/>
+      <c r="V39" s="147"/>
+      <c r="W39" s="148"/>
+      <c r="X39" s="143"/>
+      <c r="Y39" s="147"/>
+      <c r="Z39" s="147"/>
+      <c r="AA39" s="147"/>
+      <c r="AB39" s="147"/>
+      <c r="AC39" s="147"/>
+      <c r="AD39" s="148"/>
+      <c r="AE39" s="143"/>
+      <c r="AF39" s="147"/>
+      <c r="AG39" s="147"/>
+      <c r="AH39" s="147"/>
+      <c r="AI39" s="147"/>
+      <c r="AJ39" s="147"/>
+      <c r="AK39" s="148"/>
+      <c r="AL39" s="143"/>
+      <c r="AM39" s="147"/>
+      <c r="AN39" s="147"/>
+      <c r="AO39" s="147"/>
+      <c r="AP39" s="147"/>
+      <c r="AQ39" s="147"/>
+      <c r="AR39" s="148"/>
+      <c r="AS39" s="143"/>
+      <c r="AT39" s="147"/>
+      <c r="AU39" s="147"/>
+      <c r="AV39" s="147"/>
+      <c r="AW39" s="147"/>
+      <c r="AX39" s="147"/>
+      <c r="AY39" s="148"/>
+      <c r="AZ39" s="143"/>
+      <c r="BA39" s="147"/>
+      <c r="BB39" s="147"/>
+      <c r="BC39" s="147"/>
+      <c r="BD39" s="147"/>
+      <c r="BE39" s="147"/>
+      <c r="BF39" s="148"/>
+      <c r="BG39" s="143"/>
+      <c r="BH39" s="147"/>
+      <c r="BI39" s="149"/>
+      <c r="BJ39" s="149"/>
+      <c r="BK39" s="149"/>
+      <c r="BL39" s="149"/>
+      <c r="BM39" s="150"/>
       <c r="BN39" s="96"/>
       <c r="BO39" s="96"/>
     </row>
-    <row r="40" spans="1:67" ht="14.25" customHeight="1">
+    <row r="40" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
-      <c r="AD40" s="1"/>
-      <c r="AE40" s="1"/>
-      <c r="AF40" s="1"/>
-      <c r="AG40" s="1"/>
-      <c r="AH40" s="1"/>
-      <c r="AI40" s="1"/>
-      <c r="AJ40" s="1"/>
-      <c r="AK40" s="1"/>
-      <c r="AL40" s="1"/>
-      <c r="AM40" s="1"/>
-      <c r="AN40" s="1"/>
-      <c r="AO40" s="1"/>
-      <c r="AP40" s="1"/>
-      <c r="AQ40" s="1"/>
-      <c r="AR40" s="1"/>
-      <c r="AS40" s="1"/>
-      <c r="AT40" s="1"/>
-      <c r="AU40" s="1"/>
-      <c r="AV40" s="1"/>
-      <c r="AW40" s="1"/>
-      <c r="AX40" s="3"/>
-      <c r="AY40" s="96"/>
-      <c r="AZ40" s="96"/>
-      <c r="BA40" s="96"/>
-      <c r="BB40" s="96"/>
-      <c r="BC40" s="96"/>
-      <c r="BD40" s="96"/>
-      <c r="BE40" s="96"/>
-      <c r="BF40" s="96"/>
-      <c r="BG40" s="96"/>
-      <c r="BH40" s="96"/>
-      <c r="BI40" s="96"/>
-      <c r="BJ40" s="96"/>
-      <c r="BK40" s="96"/>
-      <c r="BL40" s="96"/>
-      <c r="BM40" s="96"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="130"/>
+      <c r="E40" s="130"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="70"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="75"/>
+      <c r="U40" s="75"/>
+      <c r="V40" s="75"/>
+      <c r="W40" s="76"/>
+      <c r="X40" s="70"/>
+      <c r="Y40" s="75"/>
+      <c r="Z40" s="75"/>
+      <c r="AA40" s="75"/>
+      <c r="AB40" s="75"/>
+      <c r="AC40" s="75"/>
+      <c r="AD40" s="76"/>
+      <c r="AE40" s="70"/>
+      <c r="AF40" s="75"/>
+      <c r="AG40" s="75"/>
+      <c r="AH40" s="75"/>
+      <c r="AI40" s="75"/>
+      <c r="AJ40" s="75"/>
+      <c r="AK40" s="76"/>
+      <c r="AL40" s="70"/>
+      <c r="AM40" s="75"/>
+      <c r="AN40" s="75"/>
+      <c r="AO40" s="75"/>
+      <c r="AP40" s="75"/>
+      <c r="AQ40" s="75"/>
+      <c r="AR40" s="76"/>
+      <c r="AS40" s="70"/>
+      <c r="AT40" s="75"/>
+      <c r="AU40" s="75"/>
+      <c r="AV40" s="75"/>
+      <c r="AW40" s="75"/>
+      <c r="AX40" s="75"/>
+      <c r="AY40" s="76"/>
+      <c r="AZ40" s="70"/>
+      <c r="BA40" s="75"/>
+      <c r="BB40" s="75"/>
+      <c r="BC40" s="75"/>
+      <c r="BD40" s="75"/>
+      <c r="BE40" s="75"/>
+      <c r="BF40" s="76"/>
+      <c r="BG40" s="70"/>
+      <c r="BH40" s="75"/>
+      <c r="BI40" s="87"/>
+      <c r="BJ40" s="87"/>
+      <c r="BK40" s="87"/>
+      <c r="BL40" s="87"/>
+      <c r="BM40" s="88"/>
       <c r="BN40" s="96"/>
       <c r="BO40" s="96"/>
     </row>
     <row r="41" spans="1:67" ht="14.25" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
@@ -5162,7 +5260,7 @@
       <c r="BN42" s="96"/>
       <c r="BO42" s="96"/>
     </row>
-    <row r="43" spans="1:67" ht="14.25" customHeight="1">
+    <row r="43" spans="1:67" ht="16.5" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5300,7 +5398,7 @@
       <c r="BN44" s="96"/>
       <c r="BO44" s="96"/>
     </row>
-    <row r="45" spans="1:67" ht="16.5" customHeight="1">
+    <row r="45" spans="1:67" ht="14.25" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5576,7 +5674,7 @@
       <c r="BN48" s="96"/>
       <c r="BO48" s="96"/>
     </row>
-    <row r="49" spans="1:67" ht="14.25" customHeight="1">
+    <row r="49" spans="1:67" ht="16.5" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6266,7 +6364,7 @@
       <c r="BN58" s="96"/>
       <c r="BO58" s="96"/>
     </row>
-    <row r="59" spans="1:67" ht="16.5" customHeight="1">
+    <row r="59" spans="1:67" ht="14.25" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -6542,7 +6640,7 @@
       <c r="BN62" s="96"/>
       <c r="BO62" s="96"/>
     </row>
-    <row r="63" spans="1:67" ht="14.25" customHeight="1">
+    <row r="63" spans="1:67" ht="16.5" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -69541,14 +69639,14 @@
     </row>
     <row r="976" spans="1:67" ht="14.25" customHeight="1">
       <c r="A976" s="1"/>
-      <c r="B976" s="96"/>
-      <c r="C976" s="96"/>
-      <c r="D976" s="96"/>
-      <c r="E976" s="96"/>
-      <c r="F976" s="96"/>
-      <c r="G976" s="96"/>
-      <c r="H976" s="96"/>
-      <c r="I976" s="96"/>
+      <c r="B976" s="1"/>
+      <c r="C976" s="1"/>
+      <c r="D976" s="1"/>
+      <c r="E976" s="1"/>
+      <c r="F976" s="2"/>
+      <c r="G976" s="2"/>
+      <c r="H976" s="1"/>
+      <c r="I976" s="2"/>
       <c r="J976" s="1"/>
       <c r="K976" s="1"/>
       <c r="L976" s="1"/>
@@ -69610,14 +69708,14 @@
     </row>
     <row r="977" spans="1:67" ht="14.25" customHeight="1">
       <c r="A977" s="1"/>
-      <c r="B977" s="96"/>
-      <c r="C977" s="96"/>
-      <c r="D977" s="96"/>
-      <c r="E977" s="96"/>
-      <c r="F977" s="96"/>
-      <c r="G977" s="96"/>
-      <c r="H977" s="96"/>
-      <c r="I977" s="96"/>
+      <c r="B977" s="1"/>
+      <c r="C977" s="1"/>
+      <c r="D977" s="1"/>
+      <c r="E977" s="1"/>
+      <c r="F977" s="2"/>
+      <c r="G977" s="2"/>
+      <c r="H977" s="1"/>
+      <c r="I977" s="2"/>
       <c r="J977" s="1"/>
       <c r="K977" s="1"/>
       <c r="L977" s="1"/>
@@ -69679,14 +69777,14 @@
     </row>
     <row r="978" spans="1:67" ht="14.25" customHeight="1">
       <c r="A978" s="1"/>
-      <c r="B978" s="96"/>
-      <c r="C978" s="96"/>
-      <c r="D978" s="96"/>
-      <c r="E978" s="96"/>
-      <c r="F978" s="96"/>
-      <c r="G978" s="96"/>
-      <c r="H978" s="96"/>
-      <c r="I978" s="96"/>
+      <c r="B978" s="1"/>
+      <c r="C978" s="1"/>
+      <c r="D978" s="1"/>
+      <c r="E978" s="1"/>
+      <c r="F978" s="2"/>
+      <c r="G978" s="2"/>
+      <c r="H978" s="1"/>
+      <c r="I978" s="2"/>
       <c r="J978" s="1"/>
       <c r="K978" s="1"/>
       <c r="L978" s="1"/>
@@ -69748,14 +69846,14 @@
     </row>
     <row r="979" spans="1:67" ht="14.25" customHeight="1">
       <c r="A979" s="1"/>
-      <c r="B979" s="96"/>
-      <c r="C979" s="96"/>
-      <c r="D979" s="96"/>
-      <c r="E979" s="96"/>
-      <c r="F979" s="96"/>
-      <c r="G979" s="96"/>
-      <c r="H979" s="96"/>
-      <c r="I979" s="96"/>
+      <c r="B979" s="1"/>
+      <c r="C979" s="1"/>
+      <c r="D979" s="1"/>
+      <c r="E979" s="1"/>
+      <c r="F979" s="2"/>
+      <c r="G979" s="2"/>
+      <c r="H979" s="1"/>
+      <c r="I979" s="2"/>
       <c r="J979" s="1"/>
       <c r="K979" s="1"/>
       <c r="L979" s="1"/>
@@ -69817,15 +69915,279 @@
     </row>
     <row r="980" spans="1:67" ht="14.25" customHeight="1">
       <c r="A980" s="1"/>
+      <c r="B980" s="96"/>
+      <c r="C980" s="96"/>
+      <c r="D980" s="96"/>
+      <c r="E980" s="96"/>
+      <c r="F980" s="96"/>
+      <c r="G980" s="96"/>
+      <c r="H980" s="96"/>
+      <c r="I980" s="96"/>
+      <c r="J980" s="1"/>
+      <c r="K980" s="1"/>
+      <c r="L980" s="1"/>
+      <c r="M980" s="1"/>
+      <c r="N980" s="1"/>
+      <c r="O980" s="1"/>
+      <c r="P980" s="1"/>
+      <c r="Q980" s="1"/>
+      <c r="R980" s="1"/>
+      <c r="S980" s="1"/>
+      <c r="T980" s="1"/>
+      <c r="U980" s="1"/>
+      <c r="V980" s="1"/>
+      <c r="W980" s="1"/>
+      <c r="X980" s="1"/>
+      <c r="Y980" s="1"/>
+      <c r="Z980" s="1"/>
+      <c r="AA980" s="1"/>
+      <c r="AB980" s="1"/>
+      <c r="AC980" s="1"/>
+      <c r="AD980" s="1"/>
+      <c r="AE980" s="1"/>
+      <c r="AF980" s="1"/>
+      <c r="AG980" s="1"/>
+      <c r="AH980" s="1"/>
+      <c r="AI980" s="1"/>
+      <c r="AJ980" s="1"/>
+      <c r="AK980" s="1"/>
+      <c r="AL980" s="1"/>
+      <c r="AM980" s="1"/>
+      <c r="AN980" s="1"/>
+      <c r="AO980" s="1"/>
+      <c r="AP980" s="1"/>
+      <c r="AQ980" s="1"/>
+      <c r="AR980" s="1"/>
+      <c r="AS980" s="1"/>
+      <c r="AT980" s="1"/>
+      <c r="AU980" s="1"/>
+      <c r="AV980" s="1"/>
+      <c r="AW980" s="1"/>
+      <c r="AX980" s="3"/>
+      <c r="AY980" s="96"/>
+      <c r="AZ980" s="96"/>
+      <c r="BA980" s="96"/>
+      <c r="BB980" s="96"/>
+      <c r="BC980" s="96"/>
+      <c r="BD980" s="96"/>
+      <c r="BE980" s="96"/>
+      <c r="BF980" s="96"/>
+      <c r="BG980" s="96"/>
+      <c r="BH980" s="96"/>
+      <c r="BI980" s="96"/>
+      <c r="BJ980" s="96"/>
+      <c r="BK980" s="96"/>
+      <c r="BL980" s="96"/>
+      <c r="BM980" s="96"/>
+      <c r="BN980" s="96"/>
+      <c r="BO980" s="96"/>
     </row>
     <row r="981" spans="1:67" ht="14.25" customHeight="1">
       <c r="A981" s="1"/>
+      <c r="B981" s="96"/>
+      <c r="C981" s="96"/>
+      <c r="D981" s="96"/>
+      <c r="E981" s="96"/>
+      <c r="F981" s="96"/>
+      <c r="G981" s="96"/>
+      <c r="H981" s="96"/>
+      <c r="I981" s="96"/>
+      <c r="J981" s="1"/>
+      <c r="K981" s="1"/>
+      <c r="L981" s="1"/>
+      <c r="M981" s="1"/>
+      <c r="N981" s="1"/>
+      <c r="O981" s="1"/>
+      <c r="P981" s="1"/>
+      <c r="Q981" s="1"/>
+      <c r="R981" s="1"/>
+      <c r="S981" s="1"/>
+      <c r="T981" s="1"/>
+      <c r="U981" s="1"/>
+      <c r="V981" s="1"/>
+      <c r="W981" s="1"/>
+      <c r="X981" s="1"/>
+      <c r="Y981" s="1"/>
+      <c r="Z981" s="1"/>
+      <c r="AA981" s="1"/>
+      <c r="AB981" s="1"/>
+      <c r="AC981" s="1"/>
+      <c r="AD981" s="1"/>
+      <c r="AE981" s="1"/>
+      <c r="AF981" s="1"/>
+      <c r="AG981" s="1"/>
+      <c r="AH981" s="1"/>
+      <c r="AI981" s="1"/>
+      <c r="AJ981" s="1"/>
+      <c r="AK981" s="1"/>
+      <c r="AL981" s="1"/>
+      <c r="AM981" s="1"/>
+      <c r="AN981" s="1"/>
+      <c r="AO981" s="1"/>
+      <c r="AP981" s="1"/>
+      <c r="AQ981" s="1"/>
+      <c r="AR981" s="1"/>
+      <c r="AS981" s="1"/>
+      <c r="AT981" s="1"/>
+      <c r="AU981" s="1"/>
+      <c r="AV981" s="1"/>
+      <c r="AW981" s="1"/>
+      <c r="AX981" s="3"/>
+      <c r="AY981" s="96"/>
+      <c r="AZ981" s="96"/>
+      <c r="BA981" s="96"/>
+      <c r="BB981" s="96"/>
+      <c r="BC981" s="96"/>
+      <c r="BD981" s="96"/>
+      <c r="BE981" s="96"/>
+      <c r="BF981" s="96"/>
+      <c r="BG981" s="96"/>
+      <c r="BH981" s="96"/>
+      <c r="BI981" s="96"/>
+      <c r="BJ981" s="96"/>
+      <c r="BK981" s="96"/>
+      <c r="BL981" s="96"/>
+      <c r="BM981" s="96"/>
+      <c r="BN981" s="96"/>
+      <c r="BO981" s="96"/>
     </row>
     <row r="982" spans="1:67" ht="14.25" customHeight="1">
       <c r="A982" s="1"/>
+      <c r="B982" s="96"/>
+      <c r="C982" s="96"/>
+      <c r="D982" s="96"/>
+      <c r="E982" s="96"/>
+      <c r="F982" s="96"/>
+      <c r="G982" s="96"/>
+      <c r="H982" s="96"/>
+      <c r="I982" s="96"/>
+      <c r="J982" s="1"/>
+      <c r="K982" s="1"/>
+      <c r="L982" s="1"/>
+      <c r="M982" s="1"/>
+      <c r="N982" s="1"/>
+      <c r="O982" s="1"/>
+      <c r="P982" s="1"/>
+      <c r="Q982" s="1"/>
+      <c r="R982" s="1"/>
+      <c r="S982" s="1"/>
+      <c r="T982" s="1"/>
+      <c r="U982" s="1"/>
+      <c r="V982" s="1"/>
+      <c r="W982" s="1"/>
+      <c r="X982" s="1"/>
+      <c r="Y982" s="1"/>
+      <c r="Z982" s="1"/>
+      <c r="AA982" s="1"/>
+      <c r="AB982" s="1"/>
+      <c r="AC982" s="1"/>
+      <c r="AD982" s="1"/>
+      <c r="AE982" s="1"/>
+      <c r="AF982" s="1"/>
+      <c r="AG982" s="1"/>
+      <c r="AH982" s="1"/>
+      <c r="AI982" s="1"/>
+      <c r="AJ982" s="1"/>
+      <c r="AK982" s="1"/>
+      <c r="AL982" s="1"/>
+      <c r="AM982" s="1"/>
+      <c r="AN982" s="1"/>
+      <c r="AO982" s="1"/>
+      <c r="AP982" s="1"/>
+      <c r="AQ982" s="1"/>
+      <c r="AR982" s="1"/>
+      <c r="AS982" s="1"/>
+      <c r="AT982" s="1"/>
+      <c r="AU982" s="1"/>
+      <c r="AV982" s="1"/>
+      <c r="AW982" s="1"/>
+      <c r="AX982" s="3"/>
+      <c r="AY982" s="96"/>
+      <c r="AZ982" s="96"/>
+      <c r="BA982" s="96"/>
+      <c r="BB982" s="96"/>
+      <c r="BC982" s="96"/>
+      <c r="BD982" s="96"/>
+      <c r="BE982" s="96"/>
+      <c r="BF982" s="96"/>
+      <c r="BG982" s="96"/>
+      <c r="BH982" s="96"/>
+      <c r="BI982" s="96"/>
+      <c r="BJ982" s="96"/>
+      <c r="BK982" s="96"/>
+      <c r="BL982" s="96"/>
+      <c r="BM982" s="96"/>
+      <c r="BN982" s="96"/>
+      <c r="BO982" s="96"/>
     </row>
     <row r="983" spans="1:67" ht="14.25" customHeight="1">
       <c r="A983" s="1"/>
+      <c r="B983" s="96"/>
+      <c r="C983" s="96"/>
+      <c r="D983" s="96"/>
+      <c r="E983" s="96"/>
+      <c r="F983" s="96"/>
+      <c r="G983" s="96"/>
+      <c r="H983" s="96"/>
+      <c r="I983" s="96"/>
+      <c r="J983" s="1"/>
+      <c r="K983" s="1"/>
+      <c r="L983" s="1"/>
+      <c r="M983" s="1"/>
+      <c r="N983" s="1"/>
+      <c r="O983" s="1"/>
+      <c r="P983" s="1"/>
+      <c r="Q983" s="1"/>
+      <c r="R983" s="1"/>
+      <c r="S983" s="1"/>
+      <c r="T983" s="1"/>
+      <c r="U983" s="1"/>
+      <c r="V983" s="1"/>
+      <c r="W983" s="1"/>
+      <c r="X983" s="1"/>
+      <c r="Y983" s="1"/>
+      <c r="Z983" s="1"/>
+      <c r="AA983" s="1"/>
+      <c r="AB983" s="1"/>
+      <c r="AC983" s="1"/>
+      <c r="AD983" s="1"/>
+      <c r="AE983" s="1"/>
+      <c r="AF983" s="1"/>
+      <c r="AG983" s="1"/>
+      <c r="AH983" s="1"/>
+      <c r="AI983" s="1"/>
+      <c r="AJ983" s="1"/>
+      <c r="AK983" s="1"/>
+      <c r="AL983" s="1"/>
+      <c r="AM983" s="1"/>
+      <c r="AN983" s="1"/>
+      <c r="AO983" s="1"/>
+      <c r="AP983" s="1"/>
+      <c r="AQ983" s="1"/>
+      <c r="AR983" s="1"/>
+      <c r="AS983" s="1"/>
+      <c r="AT983" s="1"/>
+      <c r="AU983" s="1"/>
+      <c r="AV983" s="1"/>
+      <c r="AW983" s="1"/>
+      <c r="AX983" s="3"/>
+      <c r="AY983" s="96"/>
+      <c r="AZ983" s="96"/>
+      <c r="BA983" s="96"/>
+      <c r="BB983" s="96"/>
+      <c r="BC983" s="96"/>
+      <c r="BD983" s="96"/>
+      <c r="BE983" s="96"/>
+      <c r="BF983" s="96"/>
+      <c r="BG983" s="96"/>
+      <c r="BH983" s="96"/>
+      <c r="BI983" s="96"/>
+      <c r="BJ983" s="96"/>
+      <c r="BK983" s="96"/>
+      <c r="BL983" s="96"/>
+      <c r="BM983" s="96"/>
+      <c r="BN983" s="96"/>
+      <c r="BO983" s="96"/>
     </row>
     <row r="984" spans="1:67" ht="14.25" customHeight="1">
       <c r="A984" s="1"/>
@@ -70076,25 +70438,36 @@
     <row r="1066" spans="1:1" ht="14.25" customHeight="1">
       <c r="A1066" s="1"/>
     </row>
+    <row r="1067" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A1067" s="1"/>
+    </row>
+    <row r="1068" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A1068" s="1"/>
+    </row>
+    <row r="1069" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A1069" s="1"/>
+    </row>
+    <row r="1070" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A1070" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B11:E13"/>
+  <mergeCells count="44">
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="BB10:BC10"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="AL11:AR11"/>
+    <mergeCell ref="AS11:AY11"/>
+    <mergeCell ref="AZ11:BF11"/>
+    <mergeCell ref="BG11:BM11"/>
+    <mergeCell ref="K10:Z10"/>
+    <mergeCell ref="AE11:AK11"/>
+    <mergeCell ref="Q11:W11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="X11:AD11"/>
     <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C26:E26"/>
@@ -70108,19 +70481,25 @@
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="AL11:AR11"/>
-    <mergeCell ref="AS11:AY11"/>
-    <mergeCell ref="AZ11:BF11"/>
-    <mergeCell ref="BG11:BM11"/>
-    <mergeCell ref="K10:Z10"/>
-    <mergeCell ref="AE11:AK11"/>
-    <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="X11:AD11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I14:I36" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I14:I40">
       <formula1>$I$3:$I$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update WBS and Sprint Backlog from Sprint 2
</commit_message>
<xml_diff>
--- a/project/Work breakdown structure.xlsx
+++ b/project/Work breakdown structure.xlsx
@@ -372,7 +372,7 @@
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,8 +443,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,6 +546,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1110,10 +1122,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1405,29 +1418,99 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1495,96 +1578,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="20" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1803,9 +1818,9 @@
   </sheetPr>
   <dimension ref="A1:BO1070"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BE10" sqref="BE10"/>
+      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -1906,12 +1921,12 @@
     </row>
     <row r="2" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="131"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
@@ -2190,10 +2205,10 @@
     </row>
     <row r="6" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="114"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
@@ -2488,24 +2503,24 @@
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="142" t="s">
+      <c r="K10" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="142"/>
-      <c r="R10" s="142"/>
-      <c r="S10" s="142"/>
-      <c r="T10" s="142"/>
-      <c r="U10" s="142"/>
-      <c r="V10" s="142"/>
-      <c r="W10" s="142"/>
-      <c r="X10" s="142"/>
-      <c r="Y10" s="142"/>
-      <c r="Z10" s="142"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="112"/>
+      <c r="P10" s="112"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="112"/>
+      <c r="V10" s="112"/>
+      <c r="W10" s="112"/>
+      <c r="X10" s="112"/>
+      <c r="Y10" s="112"/>
+      <c r="Z10" s="112"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -2533,10 +2548,10 @@
       <c r="AY10" s="96"/>
       <c r="AZ10" s="96"/>
       <c r="BA10" s="96"/>
-      <c r="BB10" s="142" t="s">
+      <c r="BB10" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="BC10" s="142"/>
+      <c r="BC10" s="112"/>
       <c r="BD10" s="96"/>
       <c r="BE10" s="96"/>
       <c r="BF10" s="96"/>
@@ -2552,109 +2567,109 @@
     </row>
     <row r="11" spans="1:67" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="97" t="s">
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="151" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="100" t="s">
+      <c r="I11" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="136" t="s">
+      <c r="J11" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="138"/>
-      <c r="Q11" s="136" t="s">
+      <c r="K11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="115"/>
+      <c r="N11" s="115"/>
+      <c r="O11" s="115"/>
+      <c r="P11" s="116"/>
+      <c r="Q11" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="R11" s="137"/>
-      <c r="S11" s="137"/>
-      <c r="T11" s="137"/>
-      <c r="U11" s="137"/>
-      <c r="V11" s="137"/>
-      <c r="W11" s="138"/>
-      <c r="X11" s="136" t="s">
+      <c r="R11" s="115"/>
+      <c r="S11" s="115"/>
+      <c r="T11" s="115"/>
+      <c r="U11" s="115"/>
+      <c r="V11" s="115"/>
+      <c r="W11" s="116"/>
+      <c r="X11" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="Y11" s="137"/>
-      <c r="Z11" s="137"/>
-      <c r="AA11" s="137"/>
-      <c r="AB11" s="137"/>
-      <c r="AC11" s="137"/>
-      <c r="AD11" s="138"/>
-      <c r="AE11" s="136" t="s">
+      <c r="Y11" s="115"/>
+      <c r="Z11" s="115"/>
+      <c r="AA11" s="115"/>
+      <c r="AB11" s="115"/>
+      <c r="AC11" s="115"/>
+      <c r="AD11" s="116"/>
+      <c r="AE11" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="AF11" s="137"/>
-      <c r="AG11" s="137"/>
-      <c r="AH11" s="137"/>
-      <c r="AI11" s="137"/>
-      <c r="AJ11" s="137"/>
-      <c r="AK11" s="138"/>
-      <c r="AL11" s="136" t="s">
+      <c r="AF11" s="115"/>
+      <c r="AG11" s="115"/>
+      <c r="AH11" s="115"/>
+      <c r="AI11" s="115"/>
+      <c r="AJ11" s="115"/>
+      <c r="AK11" s="116"/>
+      <c r="AL11" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="AM11" s="137"/>
-      <c r="AN11" s="137"/>
-      <c r="AO11" s="137"/>
-      <c r="AP11" s="137"/>
-      <c r="AQ11" s="137"/>
-      <c r="AR11" s="138"/>
-      <c r="AS11" s="136" t="s">
+      <c r="AM11" s="115"/>
+      <c r="AN11" s="115"/>
+      <c r="AO11" s="115"/>
+      <c r="AP11" s="115"/>
+      <c r="AQ11" s="115"/>
+      <c r="AR11" s="116"/>
+      <c r="AS11" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="AT11" s="137"/>
-      <c r="AU11" s="137"/>
-      <c r="AV11" s="137"/>
-      <c r="AW11" s="137"/>
-      <c r="AX11" s="137"/>
-      <c r="AY11" s="138"/>
-      <c r="AZ11" s="136" t="s">
+      <c r="AT11" s="115"/>
+      <c r="AU11" s="115"/>
+      <c r="AV11" s="115"/>
+      <c r="AW11" s="115"/>
+      <c r="AX11" s="115"/>
+      <c r="AY11" s="116"/>
+      <c r="AZ11" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="BA11" s="137"/>
-      <c r="BB11" s="137"/>
-      <c r="BC11" s="137"/>
-      <c r="BD11" s="137"/>
-      <c r="BE11" s="137"/>
-      <c r="BF11" s="138"/>
-      <c r="BG11" s="139" t="s">
+      <c r="BA11" s="115"/>
+      <c r="BB11" s="115"/>
+      <c r="BC11" s="115"/>
+      <c r="BD11" s="115"/>
+      <c r="BE11" s="115"/>
+      <c r="BF11" s="116"/>
+      <c r="BG11" s="117" t="s">
         <v>94</v>
       </c>
-      <c r="BH11" s="140"/>
-      <c r="BI11" s="140"/>
-      <c r="BJ11" s="140"/>
-      <c r="BK11" s="140"/>
-      <c r="BL11" s="140"/>
-      <c r="BM11" s="141"/>
+      <c r="BH11" s="118"/>
+      <c r="BI11" s="118"/>
+      <c r="BJ11" s="118"/>
+      <c r="BK11" s="118"/>
+      <c r="BL11" s="118"/>
+      <c r="BM11" s="119"/>
       <c r="BN11" s="96"/>
       <c r="BO11" s="96"/>
     </row>
     <row r="12" spans="1:67" ht="14.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="101"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="152"/>
+      <c r="H12" s="152"/>
+      <c r="I12" s="155"/>
       <c r="J12" s="24" t="s">
         <v>14</v>
       </c>
@@ -2828,14 +2843,14 @@
     </row>
     <row r="13" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="126"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="102"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="150"/>
+      <c r="F13" s="153"/>
+      <c r="G13" s="153"/>
+      <c r="H13" s="153"/>
+      <c r="I13" s="156"/>
       <c r="J13" s="26">
         <v>44510</v>
       </c>
@@ -3009,12 +3024,12 @@
     </row>
     <row r="14" spans="1:67" ht="16.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="134"/>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
@@ -3085,11 +3100,11 @@
       <c r="B15" s="61">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="115"/>
-      <c r="E15" s="116"/>
+      <c r="D15" s="139"/>
+      <c r="E15" s="140"/>
       <c r="F15" s="20">
         <v>44510</v>
       </c>
@@ -3166,11 +3181,11 @@
       <c r="B16" s="61">
         <v>1.2</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="116"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
       <c r="F16" s="20">
         <v>44510</v>
       </c>
@@ -3247,11 +3262,11 @@
       <c r="B17" s="61">
         <v>1.3</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="116"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
       <c r="F17" s="21">
         <v>44535</v>
       </c>
@@ -3328,11 +3343,11 @@
       <c r="B18" s="61">
         <v>1.4</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="115"/>
-      <c r="E18" s="116"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
       <c r="F18" s="21">
         <v>44535</v>
       </c>
@@ -3409,11 +3424,11 @@
       <c r="B19" s="62">
         <v>1.5</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="118"/>
-      <c r="E19" s="119"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="143"/>
       <c r="F19" s="21">
         <v>44535</v>
       </c>
@@ -3487,12 +3502,12 @@
     </row>
     <row r="20" spans="1:67" s="11" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="10"/>
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="113"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="137"/>
       <c r="F20" s="41"/>
       <c r="G20" s="33"/>
       <c r="H20" s="34"/>
@@ -3561,11 +3576,11 @@
       <c r="B21" s="15">
         <v>2.0099999999999998</v>
       </c>
-      <c r="C21" s="103" t="s">
+      <c r="C21" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="103"/>
-      <c r="E21" s="104"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="123"/>
       <c r="F21" s="36">
         <v>44527</v>
       </c>
@@ -3642,11 +3657,11 @@
       <c r="B22" s="15">
         <v>2.02</v>
       </c>
-      <c r="C22" s="103" t="s">
+      <c r="C22" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="103"/>
-      <c r="E22" s="104"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="123"/>
       <c r="F22" s="36">
         <v>44527</v>
       </c>
@@ -3723,11 +3738,11 @@
       <c r="B23" s="15">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="123"/>
       <c r="F23" s="36">
         <v>44533</v>
       </c>
@@ -3804,11 +3819,11 @@
       <c r="B24" s="15">
         <v>2.04</v>
       </c>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="103"/>
-      <c r="E24" s="104"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="123"/>
       <c r="F24" s="36">
         <v>44533</v>
       </c>
@@ -3885,11 +3900,11 @@
       <c r="B25" s="15">
         <v>2.0499999999999998</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="103"/>
-      <c r="E25" s="104"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="123"/>
       <c r="F25" s="36">
         <v>44533</v>
       </c>
@@ -3966,11 +3981,11 @@
       <c r="B26" s="15">
         <v>2.06</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="103"/>
-      <c r="E26" s="104"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="123"/>
       <c r="F26" s="36">
         <v>44535</v>
       </c>
@@ -4047,11 +4062,11 @@
       <c r="B27" s="15">
         <v>2.0699999999999998</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="103"/>
-      <c r="E27" s="104"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="123"/>
       <c r="F27" s="36">
         <v>44535</v>
       </c>
@@ -4128,11 +4143,11 @@
       <c r="B28" s="15">
         <v>2.08</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
+      <c r="D28" s="122"/>
+      <c r="E28" s="123"/>
       <c r="F28" s="36">
         <v>44535</v>
       </c>
@@ -4209,11 +4224,11 @@
       <c r="B29" s="15">
         <v>2.09</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="104"/>
+      <c r="D29" s="122"/>
+      <c r="E29" s="123"/>
       <c r="F29" s="36">
         <v>44535</v>
       </c>
@@ -4290,11 +4305,11 @@
       <c r="B30" s="15">
         <v>2.1</v>
       </c>
-      <c r="C30" s="131" t="s">
+      <c r="C30" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="125"/>
       <c r="F30" s="36">
         <v>44535</v>
       </c>
@@ -4368,14 +4383,14 @@
     </row>
     <row r="31" spans="1:67" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A31" s="10"/>
-      <c r="B31" s="155" t="s">
+      <c r="B31" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="125"/>
       <c r="F31" s="36">
         <v>44536</v>
       </c>
@@ -4449,12 +4464,12 @@
     </row>
     <row r="32" spans="1:67" ht="14.25" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="133" t="s">
+      <c r="B32" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="135"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="128"/>
       <c r="F32" s="41"/>
       <c r="G32" s="33"/>
       <c r="H32" s="34"/>
@@ -4523,11 +4538,11 @@
       <c r="B33" s="63">
         <v>3.01</v>
       </c>
-      <c r="C33" s="127" t="s">
+      <c r="C33" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="128"/>
-      <c r="E33" s="128"/>
+      <c r="D33" s="110"/>
+      <c r="E33" s="110"/>
       <c r="F33" s="64">
         <v>44545</v>
       </c>
@@ -4604,11 +4619,11 @@
       <c r="B34" s="63">
         <v>3.02</v>
       </c>
-      <c r="C34" s="127" t="s">
+      <c r="C34" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="128"/>
-      <c r="E34" s="128"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="110"/>
       <c r="F34" s="64">
         <v>44545</v>
       </c>
@@ -4685,11 +4700,11 @@
       <c r="B35" s="63">
         <v>3.03</v>
       </c>
-      <c r="C35" s="127" t="s">
+      <c r="C35" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
       <c r="F35" s="64">
         <v>44545</v>
       </c>
@@ -4763,302 +4778,302 @@
     </row>
     <row r="36" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A36" s="10"/>
-      <c r="B36" s="143">
+      <c r="B36" s="97">
         <v>3.1</v>
       </c>
-      <c r="C36" s="154" t="s">
+      <c r="C36" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="128"/>
-      <c r="E36" s="151"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="146"/>
-      <c r="I36" s="153"/>
-      <c r="J36" s="152"/>
-      <c r="K36" s="147"/>
-      <c r="L36" s="147"/>
-      <c r="M36" s="147"/>
-      <c r="N36" s="147"/>
-      <c r="O36" s="147"/>
-      <c r="P36" s="148"/>
-      <c r="Q36" s="143"/>
-      <c r="R36" s="147"/>
-      <c r="S36" s="147"/>
-      <c r="T36" s="147"/>
-      <c r="U36" s="147"/>
-      <c r="V36" s="147"/>
-      <c r="W36" s="148"/>
-      <c r="X36" s="143"/>
-      <c r="Y36" s="147"/>
-      <c r="Z36" s="147"/>
-      <c r="AA36" s="147"/>
-      <c r="AB36" s="147"/>
-      <c r="AC36" s="147"/>
-      <c r="AD36" s="148"/>
-      <c r="AE36" s="143"/>
-      <c r="AF36" s="147"/>
-      <c r="AG36" s="147"/>
-      <c r="AH36" s="147"/>
-      <c r="AI36" s="147"/>
-      <c r="AJ36" s="147"/>
-      <c r="AK36" s="148"/>
-      <c r="AL36" s="143"/>
-      <c r="AM36" s="147"/>
-      <c r="AN36" s="147"/>
-      <c r="AO36" s="147"/>
-      <c r="AP36" s="147"/>
-      <c r="AQ36" s="147"/>
-      <c r="AR36" s="148"/>
-      <c r="AS36" s="143"/>
-      <c r="AT36" s="147"/>
-      <c r="AU36" s="147"/>
-      <c r="AV36" s="147"/>
-      <c r="AW36" s="147"/>
-      <c r="AX36" s="147"/>
-      <c r="AY36" s="148"/>
-      <c r="AZ36" s="143"/>
-      <c r="BA36" s="147"/>
-      <c r="BB36" s="147"/>
-      <c r="BC36" s="147"/>
-      <c r="BD36" s="147"/>
-      <c r="BE36" s="147"/>
-      <c r="BF36" s="148"/>
-      <c r="BG36" s="143"/>
-      <c r="BH36" s="147"/>
-      <c r="BI36" s="149"/>
-      <c r="BJ36" s="149"/>
-      <c r="BK36" s="149"/>
-      <c r="BL36" s="149"/>
-      <c r="BM36" s="150"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="111"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="105"/>
+      <c r="K36" s="101"/>
+      <c r="L36" s="101"/>
+      <c r="M36" s="101"/>
+      <c r="N36" s="101"/>
+      <c r="O36" s="101"/>
+      <c r="P36" s="102"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="101"/>
+      <c r="S36" s="101"/>
+      <c r="T36" s="101"/>
+      <c r="U36" s="101"/>
+      <c r="V36" s="101"/>
+      <c r="W36" s="102"/>
+      <c r="X36" s="97"/>
+      <c r="Y36" s="101"/>
+      <c r="Z36" s="101"/>
+      <c r="AA36" s="101"/>
+      <c r="AB36" s="101"/>
+      <c r="AC36" s="101"/>
+      <c r="AD36" s="102"/>
+      <c r="AE36" s="97"/>
+      <c r="AF36" s="101"/>
+      <c r="AG36" s="101"/>
+      <c r="AH36" s="101"/>
+      <c r="AI36" s="101"/>
+      <c r="AJ36" s="101"/>
+      <c r="AK36" s="102"/>
+      <c r="AL36" s="97"/>
+      <c r="AM36" s="101"/>
+      <c r="AN36" s="101"/>
+      <c r="AO36" s="101"/>
+      <c r="AP36" s="101"/>
+      <c r="AQ36" s="101"/>
+      <c r="AR36" s="102"/>
+      <c r="AS36" s="97"/>
+      <c r="AT36" s="101"/>
+      <c r="AU36" s="101"/>
+      <c r="AV36" s="101"/>
+      <c r="AW36" s="101"/>
+      <c r="AX36" s="101"/>
+      <c r="AY36" s="102"/>
+      <c r="AZ36" s="97"/>
+      <c r="BA36" s="101"/>
+      <c r="BB36" s="101"/>
+      <c r="BC36" s="101"/>
+      <c r="BD36" s="101"/>
+      <c r="BE36" s="101"/>
+      <c r="BF36" s="102"/>
+      <c r="BG36" s="97"/>
+      <c r="BH36" s="101"/>
+      <c r="BI36" s="103"/>
+      <c r="BJ36" s="103"/>
+      <c r="BK36" s="103"/>
+      <c r="BL36" s="103"/>
+      <c r="BM36" s="104"/>
       <c r="BN36" s="96"/>
       <c r="BO36" s="96"/>
     </row>
     <row r="37" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A37" s="10"/>
-      <c r="B37" s="156" t="s">
+      <c r="B37" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="154" t="s">
+      <c r="C37" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="128"/>
-      <c r="E37" s="151"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="146"/>
-      <c r="I37" s="153" t="s">
+      <c r="D37" s="110"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="99"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="J37" s="152"/>
-      <c r="K37" s="147"/>
-      <c r="L37" s="147"/>
-      <c r="M37" s="147"/>
-      <c r="N37" s="147"/>
-      <c r="O37" s="147"/>
-      <c r="P37" s="148"/>
-      <c r="Q37" s="143"/>
-      <c r="R37" s="147"/>
-      <c r="S37" s="147"/>
-      <c r="T37" s="147"/>
-      <c r="U37" s="147"/>
-      <c r="V37" s="147"/>
-      <c r="W37" s="148"/>
-      <c r="X37" s="143"/>
-      <c r="Y37" s="147"/>
-      <c r="Z37" s="147"/>
-      <c r="AA37" s="147"/>
-      <c r="AB37" s="147"/>
-      <c r="AC37" s="147"/>
-      <c r="AD37" s="148"/>
-      <c r="AE37" s="143"/>
-      <c r="AF37" s="147"/>
-      <c r="AG37" s="147"/>
-      <c r="AH37" s="147"/>
-      <c r="AI37" s="147"/>
-      <c r="AJ37" s="147"/>
-      <c r="AK37" s="148"/>
-      <c r="AL37" s="143"/>
-      <c r="AM37" s="147"/>
-      <c r="AN37" s="147"/>
-      <c r="AO37" s="147"/>
-      <c r="AP37" s="147"/>
-      <c r="AQ37" s="147"/>
-      <c r="AR37" s="148"/>
-      <c r="AS37" s="143"/>
-      <c r="AT37" s="147"/>
-      <c r="AU37" s="147"/>
-      <c r="AV37" s="147"/>
-      <c r="AW37" s="147"/>
-      <c r="AX37" s="147"/>
-      <c r="AY37" s="148"/>
-      <c r="AZ37" s="143"/>
-      <c r="BA37" s="147"/>
-      <c r="BB37" s="147"/>
-      <c r="BC37" s="147"/>
+      <c r="J37" s="105"/>
+      <c r="K37" s="101"/>
+      <c r="L37" s="101"/>
+      <c r="M37" s="101"/>
+      <c r="N37" s="101"/>
+      <c r="O37" s="101"/>
+      <c r="P37" s="102"/>
+      <c r="Q37" s="97"/>
+      <c r="R37" s="101"/>
+      <c r="S37" s="101"/>
+      <c r="T37" s="101"/>
+      <c r="U37" s="101"/>
+      <c r="V37" s="101"/>
+      <c r="W37" s="102"/>
+      <c r="X37" s="97"/>
+      <c r="Y37" s="101"/>
+      <c r="Z37" s="101"/>
+      <c r="AA37" s="101"/>
+      <c r="AB37" s="101"/>
+      <c r="AC37" s="101"/>
+      <c r="AD37" s="102"/>
+      <c r="AE37" s="97"/>
+      <c r="AF37" s="101"/>
+      <c r="AG37" s="101"/>
+      <c r="AH37" s="101"/>
+      <c r="AI37" s="101"/>
+      <c r="AJ37" s="101"/>
+      <c r="AK37" s="102"/>
+      <c r="AL37" s="97"/>
+      <c r="AM37" s="101"/>
+      <c r="AN37" s="101"/>
+      <c r="AO37" s="101"/>
+      <c r="AP37" s="101"/>
+      <c r="AQ37" s="101"/>
+      <c r="AR37" s="102"/>
+      <c r="AS37" s="97"/>
+      <c r="AT37" s="101"/>
+      <c r="AU37" s="101"/>
+      <c r="AV37" s="101"/>
+      <c r="AW37" s="101"/>
+      <c r="AX37" s="101"/>
+      <c r="AY37" s="102"/>
+      <c r="AZ37" s="97"/>
+      <c r="BA37" s="101"/>
+      <c r="BB37" s="101"/>
+      <c r="BC37" s="101"/>
       <c r="BD37" s="94"/>
       <c r="BE37" s="94"/>
       <c r="BF37" s="94"/>
       <c r="BG37" s="94"/>
-      <c r="BH37" s="147"/>
-      <c r="BI37" s="149"/>
-      <c r="BJ37" s="149"/>
-      <c r="BK37" s="149"/>
-      <c r="BL37" s="149"/>
-      <c r="BM37" s="150"/>
+      <c r="BH37" s="101"/>
+      <c r="BI37" s="103"/>
+      <c r="BJ37" s="103"/>
+      <c r="BK37" s="103"/>
+      <c r="BL37" s="103"/>
+      <c r="BM37" s="104"/>
       <c r="BN37" s="96"/>
       <c r="BO37" s="96"/>
     </row>
     <row r="38" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="10"/>
-      <c r="B38" s="156" t="s">
+      <c r="B38" s="108" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="154" t="s">
+      <c r="C38" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="128"/>
-      <c r="E38" s="151"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="146"/>
-      <c r="I38" s="153" t="s">
+      <c r="D38" s="110"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="100"/>
+      <c r="I38" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="J38" s="152"/>
-      <c r="K38" s="147"/>
-      <c r="L38" s="147"/>
-      <c r="M38" s="147"/>
-      <c r="N38" s="147"/>
-      <c r="O38" s="147"/>
-      <c r="P38" s="148"/>
-      <c r="Q38" s="143"/>
-      <c r="R38" s="147"/>
-      <c r="S38" s="147"/>
-      <c r="T38" s="147"/>
-      <c r="U38" s="147"/>
-      <c r="V38" s="147"/>
-      <c r="W38" s="148"/>
-      <c r="X38" s="143"/>
-      <c r="Y38" s="147"/>
-      <c r="Z38" s="147"/>
-      <c r="AA38" s="147"/>
-      <c r="AB38" s="147"/>
-      <c r="AC38" s="147"/>
-      <c r="AD38" s="148"/>
-      <c r="AE38" s="143"/>
-      <c r="AF38" s="147"/>
-      <c r="AG38" s="147"/>
-      <c r="AH38" s="147"/>
-      <c r="AI38" s="147"/>
-      <c r="AJ38" s="147"/>
-      <c r="AK38" s="148"/>
-      <c r="AL38" s="143"/>
-      <c r="AM38" s="147"/>
-      <c r="AN38" s="147"/>
-      <c r="AO38" s="147"/>
-      <c r="AP38" s="147"/>
-      <c r="AQ38" s="147"/>
-      <c r="AR38" s="148"/>
-      <c r="AS38" s="143"/>
-      <c r="AT38" s="147"/>
-      <c r="AU38" s="147"/>
-      <c r="AV38" s="147"/>
-      <c r="AW38" s="147"/>
-      <c r="AX38" s="147"/>
-      <c r="AY38" s="148"/>
-      <c r="AZ38" s="143"/>
-      <c r="BA38" s="147"/>
-      <c r="BB38" s="147"/>
-      <c r="BC38" s="147"/>
+      <c r="J38" s="105"/>
+      <c r="K38" s="101"/>
+      <c r="L38" s="101"/>
+      <c r="M38" s="101"/>
+      <c r="N38" s="101"/>
+      <c r="O38" s="101"/>
+      <c r="P38" s="102"/>
+      <c r="Q38" s="97"/>
+      <c r="R38" s="101"/>
+      <c r="S38" s="101"/>
+      <c r="T38" s="101"/>
+      <c r="U38" s="101"/>
+      <c r="V38" s="101"/>
+      <c r="W38" s="102"/>
+      <c r="X38" s="97"/>
+      <c r="Y38" s="101"/>
+      <c r="Z38" s="101"/>
+      <c r="AA38" s="101"/>
+      <c r="AB38" s="101"/>
+      <c r="AC38" s="101"/>
+      <c r="AD38" s="102"/>
+      <c r="AE38" s="97"/>
+      <c r="AF38" s="101"/>
+      <c r="AG38" s="101"/>
+      <c r="AH38" s="101"/>
+      <c r="AI38" s="101"/>
+      <c r="AJ38" s="101"/>
+      <c r="AK38" s="102"/>
+      <c r="AL38" s="97"/>
+      <c r="AM38" s="101"/>
+      <c r="AN38" s="101"/>
+      <c r="AO38" s="101"/>
+      <c r="AP38" s="101"/>
+      <c r="AQ38" s="101"/>
+      <c r="AR38" s="102"/>
+      <c r="AS38" s="97"/>
+      <c r="AT38" s="101"/>
+      <c r="AU38" s="101"/>
+      <c r="AV38" s="101"/>
+      <c r="AW38" s="101"/>
+      <c r="AX38" s="101"/>
+      <c r="AY38" s="102"/>
+      <c r="AZ38" s="97"/>
+      <c r="BA38" s="101"/>
+      <c r="BB38" s="101"/>
+      <c r="BC38" s="101"/>
       <c r="BD38" s="94"/>
       <c r="BE38" s="94"/>
       <c r="BF38" s="94"/>
       <c r="BG38" s="94"/>
-      <c r="BH38" s="147"/>
-      <c r="BI38" s="149"/>
-      <c r="BJ38" s="149"/>
-      <c r="BK38" s="149"/>
-      <c r="BL38" s="149"/>
-      <c r="BM38" s="150"/>
+      <c r="BH38" s="101"/>
+      <c r="BI38" s="103"/>
+      <c r="BJ38" s="103"/>
+      <c r="BK38" s="103"/>
+      <c r="BL38" s="103"/>
+      <c r="BM38" s="104"/>
       <c r="BN38" s="96"/>
       <c r="BO38" s="96"/>
     </row>
     <row r="39" spans="1:67" s="12" customFormat="1" ht="14.25" customHeight="1">
       <c r="A39" s="10"/>
-      <c r="B39" s="156"/>
-      <c r="C39" s="127"/>
-      <c r="D39" s="128"/>
-      <c r="E39" s="151"/>
-      <c r="F39" s="144"/>
-      <c r="G39" s="145"/>
-      <c r="H39" s="146"/>
-      <c r="I39" s="153"/>
-      <c r="J39" s="152"/>
-      <c r="K39" s="147"/>
-      <c r="L39" s="147"/>
-      <c r="M39" s="147"/>
-      <c r="N39" s="147"/>
-      <c r="O39" s="147"/>
-      <c r="P39" s="148"/>
-      <c r="Q39" s="143"/>
-      <c r="R39" s="147"/>
-      <c r="S39" s="147"/>
-      <c r="T39" s="147"/>
-      <c r="U39" s="147"/>
-      <c r="V39" s="147"/>
-      <c r="W39" s="148"/>
-      <c r="X39" s="143"/>
-      <c r="Y39" s="147"/>
-      <c r="Z39" s="147"/>
-      <c r="AA39" s="147"/>
-      <c r="AB39" s="147"/>
-      <c r="AC39" s="147"/>
-      <c r="AD39" s="148"/>
-      <c r="AE39" s="143"/>
-      <c r="AF39" s="147"/>
-      <c r="AG39" s="147"/>
-      <c r="AH39" s="147"/>
-      <c r="AI39" s="147"/>
-      <c r="AJ39" s="147"/>
-      <c r="AK39" s="148"/>
-      <c r="AL39" s="143"/>
-      <c r="AM39" s="147"/>
-      <c r="AN39" s="147"/>
-      <c r="AO39" s="147"/>
-      <c r="AP39" s="147"/>
-      <c r="AQ39" s="147"/>
-      <c r="AR39" s="148"/>
-      <c r="AS39" s="143"/>
-      <c r="AT39" s="147"/>
-      <c r="AU39" s="147"/>
-      <c r="AV39" s="147"/>
-      <c r="AW39" s="147"/>
-      <c r="AX39" s="147"/>
-      <c r="AY39" s="148"/>
-      <c r="AZ39" s="143"/>
-      <c r="BA39" s="147"/>
-      <c r="BB39" s="147"/>
-      <c r="BC39" s="147"/>
-      <c r="BD39" s="147"/>
-      <c r="BE39" s="147"/>
-      <c r="BF39" s="148"/>
-      <c r="BG39" s="143"/>
-      <c r="BH39" s="147"/>
-      <c r="BI39" s="149"/>
-      <c r="BJ39" s="149"/>
-      <c r="BK39" s="149"/>
-      <c r="BL39" s="149"/>
-      <c r="BM39" s="150"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="110"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="105"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="101"/>
+      <c r="M39" s="101"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="101"/>
+      <c r="P39" s="102"/>
+      <c r="Q39" s="97"/>
+      <c r="R39" s="101"/>
+      <c r="S39" s="101"/>
+      <c r="T39" s="101"/>
+      <c r="U39" s="101"/>
+      <c r="V39" s="101"/>
+      <c r="W39" s="102"/>
+      <c r="X39" s="97"/>
+      <c r="Y39" s="101"/>
+      <c r="Z39" s="101"/>
+      <c r="AA39" s="101"/>
+      <c r="AB39" s="101"/>
+      <c r="AC39" s="101"/>
+      <c r="AD39" s="102"/>
+      <c r="AE39" s="97"/>
+      <c r="AF39" s="101"/>
+      <c r="AG39" s="101"/>
+      <c r="AH39" s="101"/>
+      <c r="AI39" s="101"/>
+      <c r="AJ39" s="101"/>
+      <c r="AK39" s="102"/>
+      <c r="AL39" s="97"/>
+      <c r="AM39" s="101"/>
+      <c r="AN39" s="101"/>
+      <c r="AO39" s="101"/>
+      <c r="AP39" s="101"/>
+      <c r="AQ39" s="101"/>
+      <c r="AR39" s="102"/>
+      <c r="AS39" s="97"/>
+      <c r="AT39" s="101"/>
+      <c r="AU39" s="101"/>
+      <c r="AV39" s="101"/>
+      <c r="AW39" s="101"/>
+      <c r="AX39" s="101"/>
+      <c r="AY39" s="102"/>
+      <c r="AZ39" s="97"/>
+      <c r="BA39" s="101"/>
+      <c r="BB39" s="101"/>
+      <c r="BC39" s="101"/>
+      <c r="BD39" s="101"/>
+      <c r="BE39" s="101"/>
+      <c r="BF39" s="102"/>
+      <c r="BG39" s="97"/>
+      <c r="BH39" s="101"/>
+      <c r="BI39" s="103"/>
+      <c r="BJ39" s="103"/>
+      <c r="BK39" s="103"/>
+      <c r="BL39" s="103"/>
+      <c r="BM39" s="104"/>
       <c r="BN39" s="96"/>
       <c r="BO39" s="96"/>
     </row>
     <row r="40" spans="1:67" ht="14.25" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
       <c r="B40" s="70"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="130"/>
-      <c r="E40" s="130"/>
+      <c r="C40" s="120"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="121"/>
       <c r="F40" s="71"/>
       <c r="G40" s="72"/>
       <c r="H40" s="73"/>
@@ -70452,21 +70467,16 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="BB10:BC10"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="AL11:AR11"/>
-    <mergeCell ref="AS11:AY11"/>
-    <mergeCell ref="AZ11:BF11"/>
-    <mergeCell ref="BG11:BM11"/>
-    <mergeCell ref="K10:Z10"/>
-    <mergeCell ref="AE11:AK11"/>
-    <mergeCell ref="Q11:W11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="X11:AD11"/>
-    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B11:E13"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C24:E24"/>
@@ -70481,16 +70491,21 @@
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B11:E13"/>
+    <mergeCell ref="BG11:BM11"/>
+    <mergeCell ref="K10:Z10"/>
+    <mergeCell ref="AE11:AK11"/>
+    <mergeCell ref="Q11:W11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="X11:AD11"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="BB10:BC10"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="AL11:AR11"/>
+    <mergeCell ref="AS11:AY11"/>
+    <mergeCell ref="AZ11:BF11"/>
+    <mergeCell ref="C35:E35"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="H11:H13"/>

</xml_diff>